<commit_message>
Corrected some formulas typos for the last spreadsheet; Added spice data
</commit_message>
<xml_diff>
--- a/final_experiments_data.xlsx
+++ b/final_experiments_data.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E726F38A-A7AF-6B4B-8552-7066F2D8F846}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97958E9B-D0C4-DD4F-8E8F-9CD0898A0C11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27100" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
+    <workbookView xWindow="51200" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy %" sheetId="1" r:id="rId1"/>
-    <sheet name="Exec. Time of Test Phase (ms)" sheetId="2" r:id="rId2"/>
-    <sheet name="Memory (MB)" sheetId="3" r:id="rId3"/>
-    <sheet name="Memory - Input Ratio" sheetId="6" r:id="rId4"/>
-    <sheet name="Datasets Attributes, Notes" sheetId="4" r:id="rId5"/>
-    <sheet name="Charts" sheetId="5" r:id="rId6"/>
+    <sheet name="Execution Time per Query (μs)" sheetId="7" r:id="rId2"/>
+    <sheet name="Exec. Time of Test Phase (ms)" sheetId="2" r:id="rId3"/>
+    <sheet name="Memory (MB)" sheetId="3" r:id="rId4"/>
+    <sheet name="Memory - Input Ratio" sheetId="6" r:id="rId5"/>
+    <sheet name="Datasets Attributes, Notes" sheetId="4" r:id="rId6"/>
+    <sheet name="Charts" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="49">
   <si>
     <t>DG</t>
   </si>
@@ -101,9 +102,6 @@
     <t>Binary Size for training data (MB)</t>
   </si>
   <si>
-    <t>CPT/+ Input binary size</t>
-  </si>
-  <si>
     <t>input data splitLength**</t>
   </si>
   <si>
@@ -126,6 +124,60 @@
   </si>
   <si>
     <t>* The minimum accuracy if not finely tuned</t>
+  </si>
+  <si>
+    <t>SPiCe0</t>
+  </si>
+  <si>
+    <t>SPiCe1</t>
+  </si>
+  <si>
+    <t>SPiCe2</t>
+  </si>
+  <si>
+    <t>SPiCe3</t>
+  </si>
+  <si>
+    <t>SPiCe4</t>
+  </si>
+  <si>
+    <t>SPiCe5</t>
+  </si>
+  <si>
+    <t>SPiCe6</t>
+  </si>
+  <si>
+    <t>SPiCe7</t>
+  </si>
+  <si>
+    <t>SPiCe8</t>
+  </si>
+  <si>
+    <t>SPiCe9</t>
+  </si>
+  <si>
+    <t>SPiCe10</t>
+  </si>
+  <si>
+    <t>SPiCe11</t>
+  </si>
+  <si>
+    <t>SPiCe12</t>
+  </si>
+  <si>
+    <t>SPiCe13</t>
+  </si>
+  <si>
+    <t>SPiCe14</t>
+  </si>
+  <si>
+    <t>SPiCe15</t>
+  </si>
+  <si>
+    <t>CPT/+ Input binary size (MB)</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -189,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -206,6 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2762,22 +2815,22 @@
                   <c:v>3.551861619471306</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.7294547004448706</c:v>
+                  <c:v>3.2063393910245401</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5518616194713054E-2</c:v>
+                  <c:v>6.7874262927926018E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16.516156530541572</c:v>
+                  <c:v>6.4442533111249123</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.39070477814184357</c:v>
+                  <c:v>4.4107335200209714E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>147.40225720805918</c:v>
+                  <c:v>3.9573700653562054</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>14.740225720805917</c:v>
+                  <c:v>3.147372891639364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2851,22 +2904,22 @@
                   <c:v>99.452125345196549</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>156.81469049965816</c:v>
+                  <c:v>134.81893725117473</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>98.208973778381605</c:v>
+                  <c:v>187.67233699571545</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>211.33576635854268</c:v>
+                  <c:v>82.4587251638564</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1552.1635277089606</c:v>
+                  <c:v>175.22641347719679</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2768.1433531349621</c:v>
+                  <c:v>74.317502661092973</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>448.95530870117307</c:v>
+                  <c:v>95.862152651377258</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2940,22 +2993,22 @@
                   <c:v>7.8851327952262977</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.80982444923945762</c:v>
+                  <c:v>2.6979055733049346</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.1311169716827831</c:v>
+                  <c:v>6.2218074350598851</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.228988518607316</c:v>
+                  <c:v>41.2293625819282</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.3442286688510614</c:v>
+                  <c:v>3.6664222385174323</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2132.8218652601295</c:v>
+                  <c:v>62.900078247999019</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.983190814885855</c:v>
+                  <c:v>10.068704098554846</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3029,22 +3082,22 @@
                   <c:v>13.639148618769813</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16.409600681957432</c:v>
+                  <c:v>54.668086616968409</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.6228988518607319</c:v>
+                  <c:v>10.577072639601806</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>41.556780947814275</c:v>
+                  <c:v>47.29250413809411</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.4753456405338445</c:v>
+                  <c:v>6.999533364442371</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2261.9675537441062</c:v>
+                  <c:v>66.708776031600877</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>39.425663976131489</c:v>
+                  <c:v>13.696398957592988</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3118,22 +3171,22 @@
                   <c:v>2.4863031336299142</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.9070477814184361</c:v>
+                  <c:v>3.3590222191685664</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.551861619471306</c:v>
+                  <c:v>6.7874262927926026</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6174201053126973</c:v>
+                  <c:v>1.8016192052607281</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.6638962146034793</c:v>
+                  <c:v>0.30073183091052075</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>39.958443219052185</c:v>
+                  <c:v>1.0727810418134291</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>10.833177939387483</c:v>
+                  <c:v>2.3131294745783277</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3207,22 +3260,22 @@
                   <c:v>1.1898736425228875</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.1311169716827831</c:v>
+                  <c:v>1.8321939377283087</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3.5518616194713054E-2</c:v>
+                  <c:v>6.7874262927926018E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.6174201053126973</c:v>
+                  <c:v>1.8016192052607281</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.14207446477885222</c:v>
+                  <c:v>1.6039030981894443E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>461.74201053126973</c:v>
+                  <c:v>12.396580927621848</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.6829785911540887</c:v>
+                  <c:v>1.2134449702705983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3298,22 +3351,22 @@
                   <c:v>19.002459664171486</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47.950131862862627</c:v>
+                  <c:v>41.224363598886953</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.6365024818633067</c:v>
+                  <c:v>14.592966529504094</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.652192830567323</c:v>
+                  <c:v>22.10448178762201</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.835637603558965</c:v>
+                  <c:v>3.3681965061978327</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>667.74998446060545</c:v>
+                  <c:v>17.927363187637749</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>115.79068879476455</c:v>
+                  <c:v>24.723941269263438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3389,22 +3442,22 @@
                   <c:v>4.0846408623920016</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3933509150483498</c:v>
+                  <c:v>5.4965818131849264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.3087100526563487</c:v>
+                  <c:v>4.4118270903151915</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.2348402106253946</c:v>
+                  <c:v>3.6032384105214561</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.685438255325572</c:v>
+                  <c:v>2.7867816331041588</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>106.02306934121847</c:v>
+                  <c:v>2.8464456976116317</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.759308097356527</c:v>
+                  <c:v>3.7920155320956193</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5248,9 +5301,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>787043</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>80492</xdr:rowOff>
+      <xdr:colOff>53663</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>143098</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="3970986" cy="3709092"/>
     <xdr:sp macro="" textlink="">
@@ -5266,7 +5319,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2897747" y="6072746"/>
+          <a:off x="2164367" y="8192394"/>
           <a:ext cx="3970986" cy="3709092"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5332,8 +5385,8 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>71550</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:colOff>661832</xdr:colOff>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>187817</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6251620" cy="2503506"/>
@@ -5350,7 +5403,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="11233240" y="4534437"/>
+          <a:off x="11823522" y="8237113"/>
           <a:ext cx="6251620" cy="2503506"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5429,10 +5482,10 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>169930</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>17888</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>545564</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>80494</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4447179" cy="1125693"/>
     <xdr:sp macro="" textlink="">
@@ -5448,7 +5501,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8040353" y="8272888"/>
+          <a:off x="6770353" y="9775424"/>
           <a:ext cx="4447179" cy="1125693"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5939,10 +5992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F97A20-C648-D746-9C76-A8398157CF72}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A10" sqref="A10:A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5950,7 +6003,7 @@
     <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="34" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5961,7 +6014,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -5982,7 +6035,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -6017,7 +6070,7 @@
         <v>0.19</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -6052,7 +6105,7 @@
         <v>3.64</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -6087,7 +6140,7 @@
         <v>29.57</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -6122,7 +6175,7 @@
         <v>2.1800000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -6157,7 +6210,7 @@
         <v>6.24</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -6192,7 +6245,7 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -6227,9 +6280,569 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3">
+        <v>67.760000000000005</v>
+      </c>
+      <c r="C10" s="3">
+        <v>61.86</v>
+      </c>
+      <c r="D10" s="3">
+        <v>67.760000000000005</v>
+      </c>
+      <c r="E10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="3">
+        <v>67.760000000000005</v>
+      </c>
+      <c r="G10" s="4">
+        <v>64</v>
+      </c>
+      <c r="H10" s="4">
+        <v>63.66</v>
+      </c>
+      <c r="I10" s="4">
+        <v>62.28</v>
+      </c>
+      <c r="J10" s="3">
+        <v>63.52</v>
+      </c>
+      <c r="K10" s="4">
+        <v>47.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3">
+        <v>26.88</v>
+      </c>
+      <c r="C11" s="3">
+        <v>8.16</v>
+      </c>
+      <c r="D11" s="3">
+        <v>26.64</v>
+      </c>
+      <c r="E11" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="3">
+        <v>26.8</v>
+      </c>
+      <c r="G11" s="4">
+        <v>25.9</v>
+      </c>
+      <c r="H11" s="4">
+        <v>26.88</v>
+      </c>
+      <c r="I11" s="4">
+        <v>15.3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>25.58</v>
+      </c>
+      <c r="K11" s="4">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3">
+        <v>36.5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>26.88</v>
+      </c>
+      <c r="D12" s="3">
+        <v>36.5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="3">
+        <v>36.5</v>
+      </c>
+      <c r="G12" s="4">
+        <v>36.4</v>
+      </c>
+      <c r="H12" s="4">
+        <v>36.5</v>
+      </c>
+      <c r="I12" s="4">
+        <v>30.82</v>
+      </c>
+      <c r="J12" s="3">
+        <v>36.380000000000003</v>
+      </c>
+      <c r="K12" s="4">
+        <v>36.799999999999997</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3">
+        <v>26.28</v>
+      </c>
+      <c r="C13" s="3">
+        <v>21.12</v>
+      </c>
+      <c r="D13" s="3">
+        <v>26.44</v>
+      </c>
       <c r="E13" t="s">
-        <v>31</v>
+        <v>48</v>
+      </c>
+      <c r="F13" s="3">
+        <v>26.52</v>
+      </c>
+      <c r="G13" s="4">
+        <v>29.1</v>
+      </c>
+      <c r="H13" s="4">
+        <v>28</v>
+      </c>
+      <c r="I13" s="4">
+        <v>27.1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>27.74</v>
+      </c>
+      <c r="K13" s="4">
+        <v>28.6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3">
+        <v>76.966999999999999</v>
+      </c>
+      <c r="C14" s="3">
+        <v>59.064999999999998</v>
+      </c>
+      <c r="D14" s="3">
+        <v>57.107999999999997</v>
+      </c>
+      <c r="E14" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="3">
+        <v>63.247</v>
+      </c>
+      <c r="G14" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="H14" s="4">
+        <v>63.658999999999999</v>
+      </c>
+      <c r="I14" s="4">
+        <v>73.671000000000006</v>
+      </c>
+      <c r="J14" s="3">
+        <v>69.055999999999997</v>
+      </c>
+      <c r="K14" s="4">
+        <v>71.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="C15" s="3">
+        <v>84.4</v>
+      </c>
+      <c r="D15" s="3">
+        <v>99.9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>48</v>
+      </c>
+      <c r="F15" s="3">
+        <v>99.94</v>
+      </c>
+      <c r="G15" s="4">
+        <v>74.5</v>
+      </c>
+      <c r="H15" s="4">
+        <v>58.66</v>
+      </c>
+      <c r="I15" s="4">
+        <v>85.56</v>
+      </c>
+      <c r="J15" s="3">
+        <v>78.819999999999993</v>
+      </c>
+      <c r="K15" s="4">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3">
+        <v>29.983000000000001</v>
+      </c>
+      <c r="C16" s="3">
+        <v>34.106000000000002</v>
+      </c>
+      <c r="D16" s="3">
+        <v>28.225999999999999</v>
+      </c>
+      <c r="E16" t="s">
+        <v>48</v>
+      </c>
+      <c r="F16" s="3">
+        <v>29.373000000000001</v>
+      </c>
+      <c r="G16" s="4">
+        <v>30.9</v>
+      </c>
+      <c r="H16" s="4">
+        <v>28.908999999999999</v>
+      </c>
+      <c r="I16" s="4">
+        <v>41.985999999999997</v>
+      </c>
+      <c r="J16" s="3">
+        <v>36.594000000000001</v>
+      </c>
+      <c r="K16" s="4">
+        <v>19.7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3">
+        <v>54.92</v>
+      </c>
+      <c r="C17" s="3">
+        <v>22.68</v>
+      </c>
+      <c r="D17" s="3">
+        <v>56.14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="3">
+        <v>56.56</v>
+      </c>
+      <c r="G17" s="4">
+        <v>57.3</v>
+      </c>
+      <c r="H17" s="4">
+        <v>54.5</v>
+      </c>
+      <c r="I17" s="4">
+        <v>25.28</v>
+      </c>
+      <c r="J17" s="3">
+        <v>44.04</v>
+      </c>
+      <c r="K17" s="4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="3">
+        <v>37.380000000000003</v>
+      </c>
+      <c r="C18" s="3">
+        <v>40.020000000000003</v>
+      </c>
+      <c r="D18" s="3">
+        <v>96.64</v>
+      </c>
+      <c r="E18" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="3">
+        <v>96.9</v>
+      </c>
+      <c r="G18" s="4">
+        <v>45.9</v>
+      </c>
+      <c r="H18" s="4">
+        <v>27.22</v>
+      </c>
+      <c r="I18" s="4">
+        <v>46.96</v>
+      </c>
+      <c r="J18" s="3">
+        <v>41.92</v>
+      </c>
+      <c r="K18" s="4">
+        <v>31.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="3">
+        <v>49.097000000000001</v>
+      </c>
+      <c r="C19" s="3">
+        <v>61.011000000000003</v>
+      </c>
+      <c r="D19" s="3">
+        <v>49.146000000000001</v>
+      </c>
+      <c r="E19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="3">
+        <v>53.344999999999999</v>
+      </c>
+      <c r="G19" s="4">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="H19" s="4">
+        <v>51.293999999999997</v>
+      </c>
+      <c r="I19" s="4">
+        <v>64.209000000000003</v>
+      </c>
+      <c r="J19" s="3">
+        <v>52.295000000000002</v>
+      </c>
+      <c r="K19" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3">
+        <v>12.98</v>
+      </c>
+      <c r="C20" s="3">
+        <v>83.5</v>
+      </c>
+      <c r="D20" s="3">
+        <v>95.94</v>
+      </c>
+      <c r="E20" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20" s="3">
+        <v>95.92</v>
+      </c>
+      <c r="G20" s="4">
+        <v>92</v>
+      </c>
+      <c r="H20" s="4">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="I20" s="4">
+        <v>86.54</v>
+      </c>
+      <c r="J20" s="3">
+        <v>82.2</v>
+      </c>
+      <c r="K20" s="4">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="3">
+        <v>48.3</v>
+      </c>
+      <c r="C21" s="3">
+        <v>13.5</v>
+      </c>
+      <c r="D21" s="3">
+        <v>90.72</v>
+      </c>
+      <c r="E21" t="s">
+        <v>48</v>
+      </c>
+      <c r="F21" s="3">
+        <v>81.739999999999995</v>
+      </c>
+      <c r="G21" s="4">
+        <v>67.3</v>
+      </c>
+      <c r="H21" s="4">
+        <v>22.68</v>
+      </c>
+      <c r="I21" s="4">
+        <v>28.68</v>
+      </c>
+      <c r="J21" s="3">
+        <v>23.76</v>
+      </c>
+      <c r="K21" s="4">
+        <v>22.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3">
+        <v>12.4</v>
+      </c>
+      <c r="C22" s="3">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="D22" s="3">
+        <v>11.34</v>
+      </c>
+      <c r="E22" t="s">
+        <v>48</v>
+      </c>
+      <c r="F22" s="3">
+        <v>12.08</v>
+      </c>
+      <c r="G22" s="4">
+        <v>12</v>
+      </c>
+      <c r="H22" s="4">
+        <v>12.58</v>
+      </c>
+      <c r="I22" s="4">
+        <v>11.32</v>
+      </c>
+      <c r="J22" s="3">
+        <v>11.94</v>
+      </c>
+      <c r="K22" s="4">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="3">
+        <v>41.92</v>
+      </c>
+      <c r="C23" s="3">
+        <v>21.52</v>
+      </c>
+      <c r="D23" s="3">
+        <v>36.9</v>
+      </c>
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+      <c r="F23" s="3">
+        <v>37.44</v>
+      </c>
+      <c r="G23" s="4">
+        <v>40</v>
+      </c>
+      <c r="H23" s="4">
+        <v>38.340000000000003</v>
+      </c>
+      <c r="I23" s="4">
+        <v>44.58</v>
+      </c>
+      <c r="J23" s="3">
+        <v>41.06</v>
+      </c>
+      <c r="K23" s="4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="3">
+        <v>59.52</v>
+      </c>
+      <c r="C24" s="3">
+        <v>73.62</v>
+      </c>
+      <c r="D24" s="3">
+        <v>55.06</v>
+      </c>
+      <c r="E24" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="3">
+        <v>55.38</v>
+      </c>
+      <c r="G24" s="4">
+        <v>58.12</v>
+      </c>
+      <c r="H24" s="4">
+        <v>59.78</v>
+      </c>
+      <c r="I24" s="4">
+        <v>75</v>
+      </c>
+      <c r="J24" s="3">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="K24" s="4">
+        <v>54.49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="3">
+        <v>27.78</v>
+      </c>
+      <c r="C25" s="3">
+        <v>33.78</v>
+      </c>
+      <c r="D25" s="3">
+        <v>24.7</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F25" s="3">
+        <v>25.82</v>
+      </c>
+      <c r="G25" s="4">
+        <v>39.5</v>
+      </c>
+      <c r="H25" s="4">
+        <v>26.68</v>
+      </c>
+      <c r="I25" s="4">
+        <v>40.340000000000003</v>
+      </c>
+      <c r="J25" s="3">
+        <v>35.74</v>
+      </c>
+      <c r="K25" s="4">
+        <v>21.5</v>
       </c>
     </row>
   </sheetData>
@@ -6239,11 +6852,346 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D61A1C-C42B-6442-B132-77D4B94522A1}">
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="29" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="2"/>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!B2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>3.2853025936599418</v>
+      </c>
+      <c r="C2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!C2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>2.4495677233429394</v>
+      </c>
+      <c r="D2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!D2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>393.37175792507207</v>
+      </c>
+      <c r="E2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!E2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>278.38616714697406</v>
+      </c>
+      <c r="F2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!F2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>1729.1066282420747</v>
+      </c>
+      <c r="G2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!G2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>1.0086455331412103</v>
+      </c>
+      <c r="H2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!H2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>3.4870317002881843</v>
+      </c>
+      <c r="I2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!I2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>9.0489913544668603</v>
+      </c>
+      <c r="J2" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!J2/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>1068884.7262247838</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!B3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>9.6153846153846168</v>
+      </c>
+      <c r="C3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!C3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>1.3461538461538463</v>
+      </c>
+      <c r="D3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!D3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>623.46153846153857</v>
+      </c>
+      <c r="E3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!E3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>792.5</v>
+      </c>
+      <c r="F3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!F3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>8076.9230769230762</v>
+      </c>
+      <c r="G3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!G3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>5.384615384615385</v>
+      </c>
+      <c r="H3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!H3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>8.0769230769230766</v>
+      </c>
+      <c r="I3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!I3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>41.15384615384616</v>
+      </c>
+      <c r="J3" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!J3/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>6730.7692307692305</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!B4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>0.78431372549019618</v>
+      </c>
+      <c r="C4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!C4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>1.4005602240896358</v>
+      </c>
+      <c r="D4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!D4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>139.21568627450981</v>
+      </c>
+      <c r="E4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!E4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>67.61904761904762</v>
+      </c>
+      <c r="F4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!F4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>330.53221288515408</v>
+      </c>
+      <c r="G4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!G4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>0</v>
+      </c>
+      <c r="H4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!H4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>1.792717086834734</v>
+      </c>
+      <c r="I4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!I4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>8.5994397759103638</v>
+      </c>
+      <c r="J4" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!J4/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>308.12324929971993</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!B5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>6.6761363636363642</v>
+      </c>
+      <c r="C5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!C5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>1.1931818181818181</v>
+      </c>
+      <c r="D5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!D5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>197.21590909090912</v>
+      </c>
+      <c r="E5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!E5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>20.085227272727273</v>
+      </c>
+      <c r="F5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!F5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>965.90909090909099</v>
+      </c>
+      <c r="G5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!G5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>3.0397727272727275</v>
+      </c>
+      <c r="H5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!H5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>2.6136363636363638</v>
+      </c>
+      <c r="I5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!I5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>50.909090909090914</v>
+      </c>
+      <c r="J5" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!J5/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!B6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>0.78431372549019618</v>
+      </c>
+      <c r="C6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!C6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>1.4005602240896358</v>
+      </c>
+      <c r="D6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!D6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>43.977591036414559</v>
+      </c>
+      <c r="E6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!E6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>20.588235294117649</v>
+      </c>
+      <c r="F6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!F6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>243.69747899159663</v>
+      </c>
+      <c r="G6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!G6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>0.39215686274509809</v>
+      </c>
+      <c r="H6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!H6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>0.58823529411764697</v>
+      </c>
+      <c r="I6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!I6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>11.596638655462185</v>
+      </c>
+      <c r="J6" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!J6/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>2156.8627450980389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!B7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>7.7784691972619786</v>
+      </c>
+      <c r="C7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!C7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>1.316116988176727</v>
+      </c>
+      <c r="D7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!D7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>1863.72121966397</v>
+      </c>
+      <c r="E7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!E7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>1834.7853142501556</v>
+      </c>
+      <c r="F7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!F7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>30214.68574984443</v>
+      </c>
+      <c r="G7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!G7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>7.4424393279402619</v>
+      </c>
+      <c r="H7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!H7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>3.0864965774735533</v>
+      </c>
+      <c r="I7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!I7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>135.03422526446795</v>
+      </c>
+      <c r="J7" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!J7/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>619985.37647790916</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!B8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>1.6056338028169013</v>
+      </c>
+      <c r="C8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!C8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>1.6056338028169013</v>
+      </c>
+      <c r="D8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!D8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>183.6901408450704</v>
+      </c>
+      <c r="E8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!E8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>42.25352112676056</v>
+      </c>
+      <c r="F8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!F8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>3352.1126760563379</v>
+      </c>
+      <c r="G8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!G8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>2.1971830985915495</v>
+      </c>
+      <c r="H8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!H8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>2.8169014084507045</v>
+      </c>
+      <c r="I8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!I8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>20.309859154929576</v>
+      </c>
+      <c r="J8" s="8">
+        <f>'Exec. Time of Test Phase (ms)'!J8/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>51107.042253521133</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BA0485-4631-4D4D-BD6C-8B9119B36FE5}">
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="O21" sqref="O21"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6506,15 +7454,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9058626D-1839-5446-B7A4-B72B5F5525AF}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6751,18 +7700,482 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="8">
+        <v>1.44E-4</v>
+      </c>
+      <c r="C10" s="8">
+        <v>6.1200960000000002</v>
+      </c>
+      <c r="D10" s="8">
+        <v>8.6183999999999997E-2</v>
+      </c>
+      <c r="E10" s="8">
+        <v>0.1739</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0.21460000000000001</v>
+      </c>
+      <c r="G10" s="8">
+        <v>1.44E-4</v>
+      </c>
+      <c r="H10" s="8">
+        <v>4.0067999999999999E-2</v>
+      </c>
+      <c r="I10" s="8">
+        <v>8.3239999999999995E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="C11" s="8">
+        <v>26.134599999999999</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0.107</v>
+      </c>
+      <c r="E11" s="8">
+        <v>0.467084</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0.64</v>
+      </c>
+      <c r="G11" s="8">
+        <v>3.2799999999999999E-3</v>
+      </c>
+      <c r="H11" s="8">
+        <v>4.0913000000000004</v>
+      </c>
+      <c r="I11" s="8">
+        <v>0.72475000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8">
+        <v>8.4000000000000003E-4</v>
+      </c>
+      <c r="C12" s="8">
+        <v>26.493300000000001</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="E12" s="8">
+        <v>0.41660000000000003</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="G12" s="8">
+        <v>8.4000000000000003E-4</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1.94767</v>
+      </c>
+      <c r="I12" s="8">
+        <v>0.59789999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C13" s="8">
+        <v>26.983000000000001</v>
+      </c>
+      <c r="D13" s="8">
+        <v>0.11</v>
+      </c>
+      <c r="E13" s="8">
+        <v>0.41899999999999998</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="G13" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="H13" s="5">
+        <v>2.0310000000000001</v>
+      </c>
+      <c r="I13" s="8">
+        <v>0.61299999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C14" s="8">
+        <v>3.6720000000000002</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0.12</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="G14" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0.26200000000000001</v>
+      </c>
+      <c r="I14" s="8">
+        <v>9.8000000000000004E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C15" s="8">
+        <v>78.534999999999997</v>
+      </c>
+      <c r="D15" s="8">
+        <v>0.106</v>
+      </c>
+      <c r="E15" s="8">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="F15" s="5">
+        <v>1.7</v>
+      </c>
+      <c r="G15" s="5">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H15" s="5">
+        <v>1.8240000000000001</v>
+      </c>
+      <c r="I15" s="8">
+        <v>1.385</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C16">
+        <v>14.763</v>
+      </c>
+      <c r="D16">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.32</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0.39</v>
+      </c>
+      <c r="G16" s="9">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1.454</v>
+      </c>
+      <c r="I16">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C17" s="8">
+        <v>37.884</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0.108</v>
+      </c>
+      <c r="E17" s="8">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0.9</v>
+      </c>
+      <c r="G17" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H17" s="5">
+        <v>3.21</v>
+      </c>
+      <c r="I17" s="8">
+        <v>0.88500000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="8">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C18" s="8">
+        <v>19.535</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0.124</v>
+      </c>
+      <c r="E18" s="8">
+        <v>0.42</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0.5</v>
+      </c>
+      <c r="G18" s="5">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="H18" s="5">
+        <v>1.54</v>
+      </c>
+      <c r="I18" s="8">
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8">
+        <v>1E-3</v>
+      </c>
+      <c r="C19" s="8">
+        <v>15.207000000000001</v>
+      </c>
+      <c r="D19" s="8">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="E19" s="8">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="F19" s="5">
+        <v>0.41</v>
+      </c>
+      <c r="G19" s="5">
+        <v>1E-3</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.504</v>
+      </c>
+      <c r="I19" s="8">
+        <v>0.23699999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C20" s="8">
+        <v>22.076000000000001</v>
+      </c>
+      <c r="D20" s="8">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="E20" s="8">
+        <v>0.253</v>
+      </c>
+      <c r="F20" s="4">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G20" s="5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H20" s="5">
+        <v>1.476</v>
+      </c>
+      <c r="I20" s="8">
+        <v>0.45100000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="8">
+        <v>0.39400000000000002</v>
+      </c>
+      <c r="C21" s="8">
+        <v>6.3929999999999998</v>
+      </c>
+      <c r="D21" s="8">
+        <v>1.4379999999999999</v>
+      </c>
+      <c r="E21" s="8">
+        <v>1.792</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0.22</v>
+      </c>
+      <c r="G21" s="5">
+        <v>0.123</v>
+      </c>
+      <c r="H21" s="5">
+        <v>1.5249999999999999</v>
+      </c>
+      <c r="I21" s="8">
+        <v>0.26800000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C22" s="8">
+        <v>20.518000000000001</v>
+      </c>
+      <c r="D22" s="8">
+        <v>0.108</v>
+      </c>
+      <c r="E22" s="8">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0.52</v>
+      </c>
+      <c r="G22" s="5">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H22" s="5">
+        <v>3.8079999999999998</v>
+      </c>
+      <c r="I22" s="8">
+        <v>0.61399999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="8">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="C23" s="8">
+        <v>3.831</v>
+      </c>
+      <c r="D23" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="E23" s="8">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="F23" s="5">
+        <v>0.15</v>
+      </c>
+      <c r="G23" s="5">
+        <v>2.7E-2</v>
+      </c>
+      <c r="H23" s="5">
+        <v>0.59</v>
+      </c>
+      <c r="I23" s="8">
+        <v>0.14599999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="8">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C24" s="8">
+        <v>26.413</v>
+      </c>
+      <c r="D24" s="8">
+        <v>0.10199999999999999</v>
+      </c>
+      <c r="E24" s="8">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="F24" s="5">
+        <v>0.65</v>
+      </c>
+      <c r="G24" s="5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H24" s="5">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="I24" s="8">
+        <v>0.35399999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="8">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C25" s="8">
+        <v>26.048999999999999</v>
+      </c>
+      <c r="D25" s="8">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="E25" s="8">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0.64400000000000002</v>
+      </c>
+      <c r="G25" s="5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="H25" s="5">
+        <v>2.4340000000000002</v>
+      </c>
+      <c r="I25" s="8">
+        <v>0.60899999999999999</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA1A666-1255-6442-A7B1-7B11C7C732E9}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="Q54" sqref="Q54"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6802,35 +8215,35 @@
         <v>8</v>
       </c>
       <c r="B2" s="8">
-        <f>'Memory (MB)'!B2/'Datasets Attributes, Notes'!$H$2</f>
+        <f>'Memory (MB)'!B2/'Datasets Attributes, Notes'!$H2</f>
         <v>3.551861619471306</v>
       </c>
       <c r="C2" s="8">
-        <f>'Memory (MB)'!C2/'Datasets Attributes, Notes'!$H$2</f>
+        <f>'Memory (MB)'!C2/'Datasets Attributes, Notes'!$H2</f>
         <v>99.452125345196549</v>
       </c>
       <c r="D2" s="8">
-        <f>'Memory (MB)'!D2/'Datasets Attributes, Notes'!$I$2</f>
+        <f>'Memory (MB)'!D2/'Datasets Attributes, Notes'!$I2</f>
         <v>7.8851327952262977</v>
       </c>
       <c r="E2" s="8">
-        <f>'Memory (MB)'!E2/'Datasets Attributes, Notes'!$I$2</f>
+        <f>'Memory (MB)'!E2/'Datasets Attributes, Notes'!$I2</f>
         <v>13.639148618769813</v>
       </c>
       <c r="F2" s="8">
-        <f>'Memory (MB)'!F2/'Datasets Attributes, Notes'!$H$2</f>
+        <f>'Memory (MB)'!F2/'Datasets Attributes, Notes'!$H2</f>
         <v>2.4863031336299142</v>
       </c>
       <c r="G2" s="8">
-        <f>'Memory (MB)'!G2/'Datasets Attributes, Notes'!$H$2</f>
+        <f>'Memory (MB)'!G2/'Datasets Attributes, Notes'!$H2</f>
         <v>1.1898736425228875</v>
       </c>
       <c r="H2" s="8">
-        <f>'Memory (MB)'!H2/'Datasets Attributes, Notes'!$H$2</f>
+        <f>'Memory (MB)'!H2/'Datasets Attributes, Notes'!$H2</f>
         <v>19.002459664171486</v>
       </c>
       <c r="I2" s="8">
-        <f>'Memory (MB)'!I2/'Datasets Attributes, Notes'!$H$2</f>
+        <f>'Memory (MB)'!I2/'Datasets Attributes, Notes'!$H2</f>
         <v>4.0846408623920016</v>
       </c>
     </row>
@@ -6839,36 +8252,36 @@
         <v>9</v>
       </c>
       <c r="B3" s="8">
-        <f>'Memory (MB)'!B3/'Datasets Attributes, Notes'!$H$2</f>
-        <v>3.7294547004448706</v>
+        <f>'Memory (MB)'!B3/'Datasets Attributes, Notes'!$H3</f>
+        <v>3.2063393910245401</v>
       </c>
       <c r="C3" s="8">
-        <f>'Memory (MB)'!C3/'Datasets Attributes, Notes'!$H$2</f>
-        <v>156.81469049965816</v>
+        <f>'Memory (MB)'!C3/'Datasets Attributes, Notes'!$H3</f>
+        <v>134.81893725117473</v>
       </c>
       <c r="D3" s="8">
-        <f>'Memory (MB)'!D3/'Datasets Attributes, Notes'!$I$2</f>
-        <v>0.80982444923945762</v>
+        <f>'Memory (MB)'!D3/'Datasets Attributes, Notes'!$I3</f>
+        <v>2.6979055733049346</v>
       </c>
       <c r="E3" s="8">
-        <f>'Memory (MB)'!E3/'Datasets Attributes, Notes'!$I$2</f>
-        <v>16.409600681957432</v>
+        <f>'Memory (MB)'!E3/'Datasets Attributes, Notes'!$I3</f>
+        <v>54.668086616968409</v>
       </c>
       <c r="F3" s="8">
-        <f>'Memory (MB)'!F3/'Datasets Attributes, Notes'!$H$2</f>
-        <v>3.9070477814184361</v>
+        <f>'Memory (MB)'!F3/'Datasets Attributes, Notes'!$H3</f>
+        <v>3.3590222191685664</v>
       </c>
       <c r="G3" s="8">
-        <f>'Memory (MB)'!G3/'Datasets Attributes, Notes'!$H$2</f>
-        <v>2.1311169716827831</v>
+        <f>'Memory (MB)'!G3/'Datasets Attributes, Notes'!$H3</f>
+        <v>1.8321939377283087</v>
       </c>
       <c r="H3" s="8">
-        <f>'Memory (MB)'!H3/'Datasets Attributes, Notes'!$H$2</f>
-        <v>47.950131862862627</v>
+        <f>'Memory (MB)'!H3/'Datasets Attributes, Notes'!$H3</f>
+        <v>41.224363598886953</v>
       </c>
       <c r="I3" s="8">
-        <f>'Memory (MB)'!I3/'Datasets Attributes, Notes'!$H$2</f>
-        <v>6.3933509150483498</v>
+        <f>'Memory (MB)'!I3/'Datasets Attributes, Notes'!$H3</f>
+        <v>5.4965818131849264</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -6876,36 +8289,36 @@
         <v>10</v>
       </c>
       <c r="B4" s="8">
-        <f>'Memory (MB)'!B4/'Datasets Attributes, Notes'!$H$2</f>
-        <v>3.5518616194713054E-2</v>
+        <f>'Memory (MB)'!B4/'Datasets Attributes, Notes'!$H4</f>
+        <v>6.7874262927926018E-2</v>
       </c>
       <c r="C4" s="8">
-        <f>'Memory (MB)'!C4/'Datasets Attributes, Notes'!$H$2</f>
-        <v>98.208973778381605</v>
+        <f>'Memory (MB)'!C4/'Datasets Attributes, Notes'!$H4</f>
+        <v>187.67233699571545</v>
       </c>
       <c r="D4" s="8">
-        <f>'Memory (MB)'!D4/'Datasets Attributes, Notes'!$I$2</f>
-        <v>2.1311169716827831</v>
+        <f>'Memory (MB)'!D4/'Datasets Attributes, Notes'!$I4</f>
+        <v>6.2218074350598851</v>
       </c>
       <c r="E4" s="8">
-        <f>'Memory (MB)'!E4/'Datasets Attributes, Notes'!$I$2</f>
-        <v>3.6228988518607319</v>
+        <f>'Memory (MB)'!E4/'Datasets Attributes, Notes'!$I4</f>
+        <v>10.577072639601806</v>
       </c>
       <c r="F4" s="8">
-        <f>'Memory (MB)'!F4/'Datasets Attributes, Notes'!$H$2</f>
-        <v>3.551861619471306</v>
+        <f>'Memory (MB)'!F4/'Datasets Attributes, Notes'!$H4</f>
+        <v>6.7874262927926026</v>
       </c>
       <c r="G4" s="8">
-        <f>'Memory (MB)'!G4/'Datasets Attributes, Notes'!$H$2</f>
-        <v>3.5518616194713054E-2</v>
+        <f>'Memory (MB)'!G4/'Datasets Attributes, Notes'!$H4</f>
+        <v>6.7874262927926018E-2</v>
       </c>
       <c r="H4" s="8">
-        <f>'Memory (MB)'!H4/'Datasets Attributes, Notes'!$H$2</f>
-        <v>7.6365024818633067</v>
+        <f>'Memory (MB)'!H4/'Datasets Attributes, Notes'!$H4</f>
+        <v>14.592966529504094</v>
       </c>
       <c r="I4" s="8">
-        <f>'Memory (MB)'!I4/'Datasets Attributes, Notes'!$H$2</f>
-        <v>2.3087100526563487</v>
+        <f>'Memory (MB)'!I4/'Datasets Attributes, Notes'!$H4</f>
+        <v>4.4118270903151915</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -6913,36 +8326,36 @@
         <v>11</v>
       </c>
       <c r="B5" s="8">
-        <f>'Memory (MB)'!B5/'Datasets Attributes, Notes'!$H$2</f>
-        <v>16.516156530541572</v>
+        <f>'Memory (MB)'!B5/'Datasets Attributes, Notes'!$H5</f>
+        <v>6.4442533111249123</v>
       </c>
       <c r="C5" s="8">
-        <f>'Memory (MB)'!C5/'Datasets Attributes, Notes'!$H$2</f>
-        <v>211.33576635854268</v>
+        <f>'Memory (MB)'!C5/'Datasets Attributes, Notes'!$H5</f>
+        <v>82.4587251638564</v>
       </c>
       <c r="D5" s="8">
-        <f>'Memory (MB)'!D5/'Datasets Attributes, Notes'!$I$2</f>
-        <v>36.228988518607316</v>
+        <f>'Memory (MB)'!D5/'Datasets Attributes, Notes'!$I5</f>
+        <v>41.2293625819282</v>
       </c>
       <c r="E5" s="8">
-        <f>'Memory (MB)'!E5/'Datasets Attributes, Notes'!$I$2</f>
-        <v>41.556780947814275</v>
+        <f>'Memory (MB)'!E5/'Datasets Attributes, Notes'!$I5</f>
+        <v>47.29250413809411</v>
       </c>
       <c r="F5" s="8">
-        <f>'Memory (MB)'!F5/'Datasets Attributes, Notes'!$H$2</f>
-        <v>4.6174201053126973</v>
+        <f>'Memory (MB)'!F5/'Datasets Attributes, Notes'!$H5</f>
+        <v>1.8016192052607281</v>
       </c>
       <c r="G5" s="8">
-        <f>'Memory (MB)'!G5/'Datasets Attributes, Notes'!$H$2</f>
-        <v>4.6174201053126973</v>
+        <f>'Memory (MB)'!G5/'Datasets Attributes, Notes'!$H5</f>
+        <v>1.8016192052607281</v>
       </c>
       <c r="H5" s="8">
-        <f>'Memory (MB)'!H5/'Datasets Attributes, Notes'!$H$2</f>
-        <v>56.652192830567323</v>
+        <f>'Memory (MB)'!H5/'Datasets Attributes, Notes'!$H5</f>
+        <v>22.10448178762201</v>
       </c>
       <c r="I5" s="8">
-        <f>'Memory (MB)'!I5/'Datasets Attributes, Notes'!$H$2</f>
-        <v>9.2348402106253946</v>
+        <f>'Memory (MB)'!I5/'Datasets Attributes, Notes'!$H5</f>
+        <v>3.6032384105214561</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -6950,36 +8363,36 @@
         <v>12</v>
       </c>
       <c r="B6" s="8">
-        <f>'Memory (MB)'!B6/'Datasets Attributes, Notes'!$H$2</f>
-        <v>0.39070477814184357</v>
+        <f>'Memory (MB)'!B6/'Datasets Attributes, Notes'!$H6</f>
+        <v>4.4107335200209714E-2</v>
       </c>
       <c r="C6" s="8">
-        <f>'Memory (MB)'!C6/'Datasets Attributes, Notes'!$H$2</f>
-        <v>1552.1635277089606</v>
+        <f>'Memory (MB)'!C6/'Datasets Attributes, Notes'!$H6</f>
+        <v>175.22641347719679</v>
       </c>
       <c r="D6" s="8">
-        <f>'Memory (MB)'!D6/'Datasets Attributes, Notes'!$I$2</f>
-        <v>2.3442286688510614</v>
+        <f>'Memory (MB)'!D6/'Datasets Attributes, Notes'!$I6</f>
+        <v>3.6664222385174323</v>
       </c>
       <c r="E6" s="8">
-        <f>'Memory (MB)'!E6/'Datasets Attributes, Notes'!$I$2</f>
-        <v>4.4753456405338445</v>
+        <f>'Memory (MB)'!E6/'Datasets Attributes, Notes'!$I6</f>
+        <v>6.999533364442371</v>
       </c>
       <c r="F6" s="8">
-        <f>'Memory (MB)'!F6/'Datasets Attributes, Notes'!$H$2</f>
-        <v>2.6638962146034793</v>
+        <f>'Memory (MB)'!F6/'Datasets Attributes, Notes'!$H6</f>
+        <v>0.30073183091052075</v>
       </c>
       <c r="G6" s="8">
-        <f>'Memory (MB)'!G6/'Datasets Attributes, Notes'!$H$2</f>
-        <v>0.14207446477885222</v>
+        <f>'Memory (MB)'!G6/'Datasets Attributes, Notes'!$H6</f>
+        <v>1.6039030981894443E-2</v>
       </c>
       <c r="H6" s="8">
-        <f>'Memory (MB)'!H6/'Datasets Attributes, Notes'!$H$2</f>
-        <v>29.835637603558965</v>
+        <f>'Memory (MB)'!H6/'Datasets Attributes, Notes'!$H6</f>
+        <v>3.3681965061978327</v>
       </c>
       <c r="I6" s="8">
-        <f>'Memory (MB)'!I6/'Datasets Attributes, Notes'!$H$2</f>
-        <v>24.685438255325572</v>
+        <f>'Memory (MB)'!I6/'Datasets Attributes, Notes'!$H6</f>
+        <v>2.7867816331041588</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -6987,36 +8400,36 @@
         <v>13</v>
       </c>
       <c r="B7" s="8">
-        <f>'Memory (MB)'!B7/'Datasets Attributes, Notes'!$H$2</f>
-        <v>147.40225720805918</v>
+        <f>'Memory (MB)'!B7/'Datasets Attributes, Notes'!$H7</f>
+        <v>3.9573700653562054</v>
       </c>
       <c r="C7" s="8">
-        <f>'Memory (MB)'!C7/'Datasets Attributes, Notes'!$H$2</f>
-        <v>2768.1433531349621</v>
+        <f>'Memory (MB)'!C7/'Datasets Attributes, Notes'!$H7</f>
+        <v>74.317502661092973</v>
       </c>
       <c r="D7" s="8">
-        <f>'Memory (MB)'!D7/'Datasets Attributes, Notes'!$I$2</f>
-        <v>2132.8218652601295</v>
+        <f>'Memory (MB)'!D7/'Datasets Attributes, Notes'!$I7</f>
+        <v>62.900078247999019</v>
       </c>
       <c r="E7" s="8">
-        <f>'Memory (MB)'!E7/'Datasets Attributes, Notes'!$I$2</f>
-        <v>2261.9675537441062</v>
+        <f>'Memory (MB)'!E7/'Datasets Attributes, Notes'!$I7</f>
+        <v>66.708776031600877</v>
       </c>
       <c r="F7" s="8">
-        <f>'Memory (MB)'!F7/'Datasets Attributes, Notes'!$H$2</f>
-        <v>39.958443219052185</v>
+        <f>'Memory (MB)'!F7/'Datasets Attributes, Notes'!$H7</f>
+        <v>1.0727810418134291</v>
       </c>
       <c r="G7" s="8">
-        <f>'Memory (MB)'!G7/'Datasets Attributes, Notes'!$H$2</f>
-        <v>461.74201053126973</v>
+        <f>'Memory (MB)'!G7/'Datasets Attributes, Notes'!$H7</f>
+        <v>12.396580927621848</v>
       </c>
       <c r="H7" s="8">
-        <f>'Memory (MB)'!H7/'Datasets Attributes, Notes'!$H$2</f>
-        <v>667.74998446060545</v>
+        <f>'Memory (MB)'!H7/'Datasets Attributes, Notes'!$H7</f>
+        <v>17.927363187637749</v>
       </c>
       <c r="I7" s="8">
-        <f>'Memory (MB)'!I7/'Datasets Attributes, Notes'!$H$2</f>
-        <v>106.02306934121847</v>
+        <f>'Memory (MB)'!I7/'Datasets Attributes, Notes'!$H7</f>
+        <v>2.8464456976116317</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -7024,49 +8437,642 @@
         <v>14</v>
       </c>
       <c r="B8" s="8">
-        <f>'Memory (MB)'!B8/'Datasets Attributes, Notes'!$H$2</f>
-        <v>14.740225720805917</v>
+        <f>'Memory (MB)'!B8/'Datasets Attributes, Notes'!$H8</f>
+        <v>3.147372891639364</v>
       </c>
       <c r="C8" s="8">
-        <f>'Memory (MB)'!C8/'Datasets Attributes, Notes'!$H$2</f>
-        <v>448.95530870117307</v>
+        <f>'Memory (MB)'!C8/'Datasets Attributes, Notes'!$H8</f>
+        <v>95.862152651377258</v>
       </c>
       <c r="D8" s="8">
-        <f>'Memory (MB)'!D8/'Datasets Attributes, Notes'!$I$2</f>
-        <v>28.983190814885855</v>
+        <f>'Memory (MB)'!D8/'Datasets Attributes, Notes'!$I8</f>
+        <v>10.068704098554846</v>
       </c>
       <c r="E8" s="8">
-        <f>'Memory (MB)'!E8/'Datasets Attributes, Notes'!$I$2</f>
-        <v>39.425663976131489</v>
+        <f>'Memory (MB)'!E8/'Datasets Attributes, Notes'!$I8</f>
+        <v>13.696398957592988</v>
       </c>
       <c r="F8" s="8">
-        <f>'Memory (MB)'!F8/'Datasets Attributes, Notes'!$H$2</f>
-        <v>10.833177939387483</v>
+        <f>'Memory (MB)'!F8/'Datasets Attributes, Notes'!$H8</f>
+        <v>2.3131294745783277</v>
       </c>
       <c r="G8" s="8">
-        <f>'Memory (MB)'!G8/'Datasets Attributes, Notes'!$H$2</f>
-        <v>5.6829785911540887</v>
+        <f>'Memory (MB)'!G8/'Datasets Attributes, Notes'!$H8</f>
+        <v>1.2134449702705983</v>
       </c>
       <c r="H8" s="8">
-        <f>'Memory (MB)'!H8/'Datasets Attributes, Notes'!$H$2</f>
-        <v>115.79068879476455</v>
+        <f>'Memory (MB)'!H8/'Datasets Attributes, Notes'!$H8</f>
+        <v>24.723941269263438</v>
       </c>
       <c r="I8" s="8">
-        <f>'Memory (MB)'!I8/'Datasets Attributes, Notes'!$H$2</f>
-        <v>17.759308097356527</v>
+        <f>'Memory (MB)'!I8/'Datasets Attributes, Notes'!$H8</f>
+        <v>3.7920155320956193</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="8">
+        <f>'Memory (MB)'!B10/'Datasets Attributes, Notes'!$H10</f>
+        <v>1.0338143441740255E-2</v>
+      </c>
+      <c r="C10" s="8">
+        <f>'Memory (MB)'!C10/'Datasets Attributes, Notes'!$H10</f>
+        <v>439.37798836958871</v>
+      </c>
+      <c r="D10" s="8">
+        <f>'Memory (MB)'!D10/'Datasets Attributes, Notes'!$I10</f>
+        <v>6.1873788498815427</v>
+      </c>
+      <c r="E10" s="8">
+        <f>'Memory (MB)'!E10/'Datasets Attributes, Notes'!$I10</f>
+        <v>12.484744059157155</v>
+      </c>
+      <c r="F10" s="8">
+        <f>'Memory (MB)'!F10/'Datasets Attributes, Notes'!$H10</f>
+        <v>15.406705434704575</v>
+      </c>
+      <c r="G10" s="8">
+        <f>'Memory (MB)'!G10/'Datasets Attributes, Notes'!$H10</f>
+        <v>1.0338143441740255E-2</v>
+      </c>
+      <c r="H10" s="8">
+        <f>'Memory (MB)'!H10/'Datasets Attributes, Notes'!$H10</f>
+        <v>2.8765884126642258</v>
+      </c>
+      <c r="I10" s="8">
+        <f>'Memory (MB)'!I10/'Datasets Attributes, Notes'!$H10</f>
+        <v>5.976021250628186</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="8">
+        <f>'Memory (MB)'!B11/'Datasets Attributes, Notes'!$H11</f>
+        <v>2.6255602391721283E-2</v>
+      </c>
+      <c r="C11" s="8">
+        <f>'Memory (MB)'!C11/'Datasets Attributes, Notes'!$H11</f>
+        <v>214.43114570833717</v>
+      </c>
+      <c r="D11" s="8">
+        <f>'Memory (MB)'!D11/'Datasets Attributes, Notes'!$I11</f>
+        <v>1.6760323458578896</v>
+      </c>
+      <c r="E11" s="8">
+        <f>'Memory (MB)'!E11/'Datasets Attributes, Notes'!$I11</f>
+        <v>7.3163354414269772</v>
+      </c>
+      <c r="F11" s="8">
+        <f>'Memory (MB)'!F11/'Datasets Attributes, Notes'!$H11</f>
+        <v>5.2511204783442569</v>
+      </c>
+      <c r="G11" s="8">
+        <f>'Memory (MB)'!G11/'Datasets Attributes, Notes'!$H11</f>
+        <v>2.6911992451514315E-2</v>
+      </c>
+      <c r="H11" s="8">
+        <f>'Memory (MB)'!H11/'Datasets Attributes, Notes'!$H11</f>
+        <v>33.568608145390399</v>
+      </c>
+      <c r="I11" s="8">
+        <f>'Memory (MB)'!I11/'Datasets Attributes, Notes'!$H11</f>
+        <v>5.9464836979374995</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="8">
+        <f>'Memory (MB)'!B12/'Datasets Attributes, Notes'!$H12</f>
+        <v>8.6151195347835465E-3</v>
+      </c>
+      <c r="C12" s="8">
+        <f>'Memory (MB)'!C12/'Datasets Attributes, Notes'!$H12</f>
+        <v>271.71779329866774</v>
+      </c>
+      <c r="D12" s="8">
+        <f>'Memory (MB)'!D12/'Datasets Attributes, Notes'!$I12</f>
+        <v>2.1537798836958864</v>
+      </c>
+      <c r="E12" s="8">
+        <f>'Memory (MB)'!E12/'Datasets Attributes, Notes'!$I12</f>
+        <v>8.156951814070057</v>
+      </c>
+      <c r="F12" s="8">
+        <f>'Memory (MB)'!F12/'Datasets Attributes, Notes'!$H12</f>
+        <v>6.6664615447729823</v>
+      </c>
+      <c r="G12" s="8">
+        <f>'Memory (MB)'!G12/'Datasets Attributes, Notes'!$H12</f>
+        <v>8.6151195347835465E-3</v>
+      </c>
+      <c r="H12" s="8">
+        <f>'Memory (MB)'!H12/'Datasets Attributes, Notes'!$H12</f>
+        <v>19.975487933704606</v>
+      </c>
+      <c r="I12" s="8">
+        <f>'Memory (MB)'!I12/'Datasets Attributes, Notes'!$H12</f>
+        <v>6.1321190117227165</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="8">
+        <f>'Memory (MB)'!B13/'Datasets Attributes, Notes'!$H13</f>
+        <v>1.0017580854399471E-2</v>
+      </c>
+      <c r="C13" s="8">
+        <f>'Memory (MB)'!C13/'Datasets Attributes, Notes'!$H13</f>
+        <v>270.30438419426093</v>
+      </c>
+      <c r="D13" s="8">
+        <f>'Memory (MB)'!D13/'Datasets Attributes, Notes'!$I13</f>
+        <v>2.1537798836958864</v>
+      </c>
+      <c r="E13" s="8">
+        <f>'Memory (MB)'!E13/'Datasets Attributes, Notes'!$I13</f>
+        <v>8.2039433751688762</v>
+      </c>
+      <c r="F13" s="8">
+        <f>'Memory (MB)'!F13/'Datasets Attributes, Notes'!$H13</f>
+        <v>6.5114275553596563</v>
+      </c>
+      <c r="G13" s="8">
+        <f>'Memory (MB)'!G13/'Datasets Attributes, Notes'!$H13</f>
+        <v>1.0017580854399471E-2</v>
+      </c>
+      <c r="H13" s="8">
+        <f>'Memory (MB)'!H13/'Datasets Attributes, Notes'!$H13</f>
+        <v>20.345706715285328</v>
+      </c>
+      <c r="I13" s="8">
+        <f>'Memory (MB)'!I13/'Datasets Attributes, Notes'!$H13</f>
+        <v>6.1407770637468762</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" s="8">
+        <f>'Memory (MB)'!B14/'Datasets Attributes, Notes'!$H14</f>
+        <v>0.25784271594327463</v>
+      </c>
+      <c r="C14" s="8">
+        <f>'Memory (MB)'!C14/'Datasets Attributes, Notes'!$H14</f>
+        <v>157.79974215728407</v>
+      </c>
+      <c r="D14" s="8">
+        <f>'Memory (MB)'!D14/'Datasets Attributes, Notes'!$I14</f>
+        <v>1.8752197523147245</v>
+      </c>
+      <c r="E14" s="8">
+        <f>'Memory (MB)'!E14/'Datasets Attributes, Notes'!$I14</f>
+        <v>4.0317224674766576</v>
+      </c>
+      <c r="F14" s="8">
+        <f>'Memory (MB)'!F14/'Datasets Attributes, Notes'!$H14</f>
+        <v>6.4460678985818651</v>
+      </c>
+      <c r="G14" s="8">
+        <f>'Memory (MB)'!G14/'Datasets Attributes, Notes'!$H14</f>
+        <v>0.17189514396218308</v>
+      </c>
+      <c r="H14" s="8">
+        <f>'Memory (MB)'!H14/'Datasets Attributes, Notes'!$H14</f>
+        <v>11.259131929522992</v>
+      </c>
+      <c r="I14" s="8">
+        <f>'Memory (MB)'!I14/'Datasets Attributes, Notes'!$H14</f>
+        <v>4.2114310270734858</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" s="8">
+        <f>'Memory (MB)'!B15/'Datasets Attributes, Notes'!$H15</f>
+        <v>2.6545186241629968E-2</v>
+      </c>
+      <c r="C15" s="8">
+        <f>'Memory (MB)'!C15/'Datasets Attributes, Notes'!$H15</f>
+        <v>189.52056377149179</v>
+      </c>
+      <c r="D15" s="8">
+        <f>'Memory (MB)'!D15/'Datasets Attributes, Notes'!$I15</f>
+        <v>3.8050111278627328</v>
+      </c>
+      <c r="E15" s="8">
+        <f>'Memory (MB)'!E15/'Datasets Attributes, Notes'!$I15</f>
+        <v>11.738100366142582</v>
+      </c>
+      <c r="F15" s="8">
+        <f>'Memory (MB)'!F15/'Datasets Attributes, Notes'!$H15</f>
+        <v>4.1024378737064495</v>
+      </c>
+      <c r="G15" s="8">
+        <f>'Memory (MB)'!G15/'Datasets Attributes, Notes'!$H15</f>
+        <v>1.447919249543453E-2</v>
+      </c>
+      <c r="H15" s="8">
+        <f>'Memory (MB)'!H15/'Datasets Attributes, Notes'!$H15</f>
+        <v>4.4016745186120971</v>
+      </c>
+      <c r="I15" s="8">
+        <f>'Memory (MB)'!I15/'Datasets Attributes, Notes'!$H15</f>
+        <v>3.3422802676961374</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16" s="8">
+        <f>'Memory (MB)'!B16/'Datasets Attributes, Notes'!$H16</f>
+        <v>5.6641178136505245E-2</v>
+      </c>
+      <c r="C16" s="8">
+        <f>'Memory (MB)'!C16/'Datasets Attributes, Notes'!$H16</f>
+        <v>167.23874256584537</v>
+      </c>
+      <c r="D16" s="8">
+        <f>'Memory (MB)'!D16/'Datasets Attributes, Notes'!$I16</f>
+        <v>1.3748358693133544</v>
+      </c>
+      <c r="E16" s="8">
+        <f>'Memory (MB)'!E16/'Datasets Attributes, Notes'!$I16</f>
+        <v>4.9432300919131844</v>
+      </c>
+      <c r="F16" s="8">
+        <f>'Memory (MB)'!F16/'Datasets Attributes, Notes'!$H16</f>
+        <v>4.4180118946474094</v>
+      </c>
+      <c r="G16" s="8">
+        <f>'Memory (MB)'!G16/'Datasets Attributes, Notes'!$H16</f>
+        <v>4.5312942509204195E-2</v>
+      </c>
+      <c r="H16" s="8">
+        <f>'Memory (MB)'!H16/'Datasets Attributes, Notes'!$H16</f>
+        <v>16.471254602095726</v>
+      </c>
+      <c r="I16" s="8">
+        <f>'Memory (MB)'!I16/'Datasets Attributes, Notes'!$H16</f>
+        <v>3.8516001132823567</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="8">
+        <f>'Memory (MB)'!B17/'Datasets Attributes, Notes'!$H17</f>
+        <v>1.7522277019898735E-2</v>
+      </c>
+      <c r="C17" s="8">
+        <f>'Memory (MB)'!C17/'Datasets Attributes, Notes'!$H17</f>
+        <v>221.27131420728122</v>
+      </c>
+      <c r="D17" s="8">
+        <f>'Memory (MB)'!D17/'Datasets Attributes, Notes'!$I17</f>
+        <v>1.6916961995574959</v>
+      </c>
+      <c r="E17" s="8">
+        <f>'Memory (MB)'!E17/'Datasets Attributes, Notes'!$I17</f>
+        <v>5.4040295263642228</v>
+      </c>
+      <c r="F17" s="8">
+        <f>'Memory (MB)'!F17/'Datasets Attributes, Notes'!$H17</f>
+        <v>5.2566831059696204</v>
+      </c>
+      <c r="G17" s="8">
+        <f>'Memory (MB)'!G17/'Datasets Attributes, Notes'!$H17</f>
+        <v>1.7522277019898735E-2</v>
+      </c>
+      <c r="H17" s="8">
+        <f>'Memory (MB)'!H17/'Datasets Attributes, Notes'!$H17</f>
+        <v>18.748836411291645</v>
+      </c>
+      <c r="I17" s="8">
+        <f>'Memory (MB)'!I17/'Datasets Attributes, Notes'!$H17</f>
+        <v>5.1690717208701269</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18" s="8">
+        <f>'Memory (MB)'!B18/'Datasets Attributes, Notes'!$H18</f>
+        <v>0.10189926331464408</v>
+      </c>
+      <c r="C18" s="8">
+        <f>'Memory (MB)'!C18/'Datasets Attributes, Notes'!$H18</f>
+        <v>180.96382807741566</v>
+      </c>
+      <c r="D18" s="8">
+        <f>'Memory (MB)'!D18/'Datasets Attributes, Notes'!$I18</f>
+        <v>1.6185982156259995</v>
+      </c>
+      <c r="E18" s="8">
+        <f>'Memory (MB)'!E18/'Datasets Attributes, Notes'!$I18</f>
+        <v>5.482348794862256</v>
+      </c>
+      <c r="F18" s="8">
+        <f>'Memory (MB)'!F18/'Datasets Attributes, Notes'!$H18</f>
+        <v>4.6317846961201861</v>
+      </c>
+      <c r="G18" s="8">
+        <f>'Memory (MB)'!G18/'Datasets Attributes, Notes'!$H18</f>
+        <v>7.4108555137922971E-2</v>
+      </c>
+      <c r="H18" s="8">
+        <f>'Memory (MB)'!H18/'Datasets Attributes, Notes'!$H18</f>
+        <v>14.265896864050172</v>
+      </c>
+      <c r="I18" s="8">
+        <f>'Memory (MB)'!I18/'Datasets Attributes, Notes'!$H18</f>
+        <v>4.0944976713702443</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19" s="8">
+        <f>'Memory (MB)'!B19/'Datasets Attributes, Notes'!$H19</f>
+        <v>1.4358532557972576E-2</v>
+      </c>
+      <c r="C19" s="8">
+        <f>'Memory (MB)'!C19/'Datasets Attributes, Notes'!$H19</f>
+        <v>218.35020460908896</v>
+      </c>
+      <c r="D19" s="8">
+        <f>'Memory (MB)'!D19/'Datasets Attributes, Notes'!$I19</f>
+        <v>1.4880661014626122</v>
+      </c>
+      <c r="E19" s="8">
+        <f>'Memory (MB)'!E19/'Datasets Attributes, Notes'!$I19</f>
+        <v>4.4446184872633294</v>
+      </c>
+      <c r="F19" s="8">
+        <f>'Memory (MB)'!F19/'Datasets Attributes, Notes'!$H19</f>
+        <v>5.8869983487687554</v>
+      </c>
+      <c r="G19" s="8">
+        <f>'Memory (MB)'!G19/'Datasets Attributes, Notes'!$H19</f>
+        <v>1.4358532557972576E-2</v>
+      </c>
+      <c r="H19" s="8">
+        <f>'Memory (MB)'!H19/'Datasets Attributes, Notes'!$H19</f>
+        <v>7.2367004092181784</v>
+      </c>
+      <c r="I19" s="8">
+        <f>'Memory (MB)'!I19/'Datasets Attributes, Notes'!$H19</f>
+        <v>3.4029722162395002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="8">
+        <f>'Memory (MB)'!B20/'Datasets Attributes, Notes'!$H20</f>
+        <v>2.9537552690686444E-2</v>
+      </c>
+      <c r="C20" s="8">
+        <f>'Memory (MB)'!C20/'Datasets Attributes, Notes'!$H20</f>
+        <v>217.35700439986465</v>
+      </c>
+      <c r="D20" s="8">
+        <f>'Memory (MB)'!D20/'Datasets Attributes, Notes'!$I20</f>
+        <v>1.5037299551622187</v>
+      </c>
+      <c r="E20" s="8">
+        <f>'Memory (MB)'!E20/'Datasets Attributes, Notes'!$I20</f>
+        <v>3.9629549860004305</v>
+      </c>
+      <c r="F20" s="8">
+        <f>'Memory (MB)'!F20/'Datasets Attributes, Notes'!$H20</f>
+        <v>5.51367650226147</v>
+      </c>
+      <c r="G20" s="8">
+        <f>'Memory (MB)'!G20/'Datasets Attributes, Notes'!$H20</f>
+        <v>2.9537552690686444E-2</v>
+      </c>
+      <c r="H20" s="8">
+        <f>'Memory (MB)'!H20/'Datasets Attributes, Notes'!$H20</f>
+        <v>14.53247592381773</v>
+      </c>
+      <c r="I20" s="8">
+        <f>'Memory (MB)'!I20/'Datasets Attributes, Notes'!$H20</f>
+        <v>4.4404787544998623</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="8">
+        <f>'Memory (MB)'!B21/'Datasets Attributes, Notes'!$H21</f>
+        <v>4.7143848565343296</v>
+      </c>
+      <c r="C21" s="8">
+        <f>'Memory (MB)'!C21/'Datasets Attributes, Notes'!$H21</f>
+        <v>76.495082202598894</v>
+      </c>
+      <c r="D21" s="8">
+        <f>'Memory (MB)'!D21/'Datasets Attributes, Notes'!$I21</f>
+        <v>17.206308181970471</v>
+      </c>
+      <c r="E21" s="8">
+        <f>'Memory (MB)'!E21/'Datasets Attributes, Notes'!$I21</f>
+        <v>21.442075286572379</v>
+      </c>
+      <c r="F21" s="8">
+        <f>'Memory (MB)'!F21/'Datasets Attributes, Notes'!$H21</f>
+        <v>2.6323976356283056</v>
+      </c>
+      <c r="G21" s="8">
+        <f>'Memory (MB)'!G21/'Datasets Attributes, Notes'!$H21</f>
+        <v>1.4717495871921891</v>
+      </c>
+      <c r="H21" s="8">
+        <f>'Memory (MB)'!H21/'Datasets Attributes, Notes'!$H21</f>
+        <v>18.247301792423482</v>
+      </c>
+      <c r="I21" s="8">
+        <f>'Memory (MB)'!I21/'Datasets Attributes, Notes'!$H21</f>
+        <v>3.2067389379472089</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="8">
+        <f>'Memory (MB)'!B22/'Datasets Attributes, Notes'!$H22</f>
+        <v>4.1770276532283858E-2</v>
+      </c>
+      <c r="C22" s="8">
+        <f>'Memory (MB)'!C22/'Datasets Attributes, Notes'!$H22</f>
+        <v>214.26063347235004</v>
+      </c>
+      <c r="D22" s="8">
+        <f>'Memory (MB)'!D22/'Datasets Attributes, Notes'!$I22</f>
+        <v>1.6916961995574959</v>
+      </c>
+      <c r="E22" s="8">
+        <f>'Memory (MB)'!E22/'Datasets Attributes, Notes'!$I22</f>
+        <v>7.2680281166173906</v>
+      </c>
+      <c r="F22" s="8">
+        <f>'Memory (MB)'!F22/'Datasets Attributes, Notes'!$H22</f>
+        <v>5.4301359491969015</v>
+      </c>
+      <c r="G22" s="8">
+        <f>'Memory (MB)'!G22/'Datasets Attributes, Notes'!$H22</f>
+        <v>4.1770276532283858E-2</v>
+      </c>
+      <c r="H22" s="8">
+        <f>'Memory (MB)'!H22/'Datasets Attributes, Notes'!$H22</f>
+        <v>39.765303258734228</v>
+      </c>
+      <c r="I22" s="8">
+        <f>'Memory (MB)'!I22/'Datasets Attributes, Notes'!$H22</f>
+        <v>6.4117374477055717</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="8">
+        <f>'Memory (MB)'!B23/'Datasets Attributes, Notes'!$H23</f>
+        <v>1.3879914806040157</v>
+      </c>
+      <c r="C23" s="8">
+        <f>'Memory (MB)'!C23/'Datasets Attributes, Notes'!$H23</f>
+        <v>91.679230382654893</v>
+      </c>
+      <c r="D23" s="8">
+        <f>'Memory (MB)'!D23/'Datasets Attributes, Notes'!$I23</f>
+        <v>7.8971929068849169</v>
+      </c>
+      <c r="E23" s="8">
+        <f>'Memory (MB)'!E23/'Datasets Attributes, Notes'!$I23</f>
+        <v>12.94661018977194</v>
+      </c>
+      <c r="F23" s="8">
+        <f>'Memory (MB)'!F23/'Datasets Attributes, Notes'!$H23</f>
+        <v>3.5896331394931438</v>
+      </c>
+      <c r="G23" s="8">
+        <f>'Memory (MB)'!G23/'Datasets Attributes, Notes'!$H23</f>
+        <v>0.64613396510876586</v>
+      </c>
+      <c r="H23" s="8">
+        <f>'Memory (MB)'!H23/'Datasets Attributes, Notes'!$H23</f>
+        <v>14.119223682006366</v>
+      </c>
+      <c r="I23" s="8">
+        <f>'Memory (MB)'!I23/'Datasets Attributes, Notes'!$H23</f>
+        <v>3.4939095891066598</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="8">
+        <f>'Memory (MB)'!B24/'Datasets Attributes, Notes'!$H24</f>
+        <v>4.9229254484477403E-2</v>
+      </c>
+      <c r="C24" s="8">
+        <f>'Memory (MB)'!C24/'Datasets Attributes, Notes'!$H24</f>
+        <v>216.71538311641694</v>
+      </c>
+      <c r="D24" s="8">
+        <f>'Memory (MB)'!D24/'Datasets Attributes, Notes'!$I24</f>
+        <v>1.5977130773598573</v>
+      </c>
+      <c r="E24" s="8">
+        <f>'Memory (MB)'!E24/'Datasets Attributes, Notes'!$I24</f>
+        <v>4.2918959136921666</v>
+      </c>
+      <c r="F24" s="8">
+        <f>'Memory (MB)'!F24/'Datasets Attributes, Notes'!$H24</f>
+        <v>5.3331692358183851</v>
+      </c>
+      <c r="G24" s="8">
+        <f>'Memory (MB)'!G24/'Datasets Attributes, Notes'!$H24</f>
+        <v>4.1024378737064507E-2</v>
+      </c>
+      <c r="H24" s="8">
+        <f>'Memory (MB)'!H24/'Datasets Attributes, Notes'!$H24</f>
+        <v>4.55370603981416</v>
+      </c>
+      <c r="I24" s="8">
+        <f>'Memory (MB)'!I24/'Datasets Attributes, Notes'!$H24</f>
+        <v>2.9045260145841665</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25" s="8">
+        <f>'Memory (MB)'!B25/'Datasets Attributes, Notes'!$H25</f>
+        <v>6.723995734465206E-2</v>
+      </c>
+      <c r="C25" s="8">
+        <f>'Memory (MB)'!C25/'Datasets Attributes, Notes'!$H25</f>
+        <v>218.94170610885519</v>
+      </c>
+      <c r="D25" s="8">
+        <f>'Memory (MB)'!D25/'Datasets Attributes, Notes'!$I25</f>
+        <v>1.8639985902531668</v>
+      </c>
+      <c r="E25" s="8">
+        <f>'Memory (MB)'!E25/'Datasets Attributes, Notes'!$I25</f>
+        <v>6.9547510426252614</v>
+      </c>
+      <c r="F25" s="8">
+        <f>'Memory (MB)'!F25/'Datasets Attributes, Notes'!$H25</f>
+        <v>5.4128165662444907</v>
+      </c>
+      <c r="G25" s="8">
+        <f>'Memory (MB)'!G25/'Datasets Attributes, Notes'!$H25</f>
+        <v>5.8834962676570554E-2</v>
+      </c>
+      <c r="H25" s="8">
+        <f>'Memory (MB)'!H25/'Datasets Attributes, Notes'!$H25</f>
+        <v>20.457757022110393</v>
+      </c>
+      <c r="I25" s="8">
+        <f>'Memory (MB)'!I25/'Datasets Attributes, Notes'!$H25</f>
+        <v>5.1186417528616381</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C2CA90-8492-FA44-8F31-E345E5B9D4A9}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:P36"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="I49" sqref="I49"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7097,10 +9103,10 @@
         <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
         <v>23</v>
-      </c>
-      <c r="N1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -7160,11 +9166,11 @@
         <v>7</v>
       </c>
       <c r="H3" s="8">
-        <f t="shared" ref="H3:H8" si="0">(_xlfn.CEILING.MATH(LOG(D3, 2))*C3)*(E3-F3)*0.000000125</f>
+        <f t="shared" ref="H3:H25" si="0">(_xlfn.CEILING.MATH(LOG(D3, 2))*C3)*(E3-F3)*0.000000125</f>
         <v>6.5495249999999991E-2</v>
       </c>
       <c r="I3" s="10">
-        <f t="shared" ref="I3:I8" si="1">(_xlfn.CEILING.MATH(LOG(D3, 2))*N3)*(E3-F3)*0.000000125</f>
+        <f t="shared" ref="I3:I25" si="1">(_xlfn.CEILING.MATH(LOG(D3, 2))*N3)*(E3-F3)*0.000000125</f>
         <v>1.4084999999999999E-2</v>
       </c>
       <c r="N3" s="11">
@@ -7341,29 +9347,594 @@
         <v>21</v>
       </c>
     </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="H9" s="8"/>
+      <c r="I9" s="10"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10">
+        <f>E10*C10</f>
+        <v>60000</v>
+      </c>
+      <c r="C10">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>5000</v>
+      </c>
+      <c r="F10">
+        <v>357</v>
+      </c>
+      <c r="G10">
+        <v>4</v>
+      </c>
+      <c r="H10" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3928999999999999E-2</v>
+      </c>
+      <c r="I10" s="10">
+        <f t="shared" si="1"/>
+        <v>1.3928999999999999E-2</v>
+      </c>
+      <c r="N10" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11:B25" si="2">E11*C11</f>
+        <v>210000</v>
+      </c>
+      <c r="C11">
+        <v>42</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>5000</v>
+      </c>
+      <c r="F11">
+        <v>357</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="0"/>
+        <v>0.12187874999999999</v>
+      </c>
+      <c r="I11" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3841250000000002E-2</v>
+      </c>
+      <c r="N11" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="2"/>
+        <v>210000</v>
+      </c>
+      <c r="C12">
+        <v>42</v>
+      </c>
+      <c r="D12">
+        <v>10</v>
+      </c>
+      <c r="E12">
+        <v>5000</v>
+      </c>
+      <c r="F12">
+        <v>357</v>
+      </c>
+      <c r="G12">
+        <v>4</v>
+      </c>
+      <c r="H12" s="8">
+        <f t="shared" si="0"/>
+        <v>9.7502999999999992E-2</v>
+      </c>
+      <c r="I12" s="10">
+        <f t="shared" si="1"/>
+        <v>5.1073E-2</v>
+      </c>
+      <c r="N12" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="2"/>
+        <v>215000</v>
+      </c>
+      <c r="C13">
+        <v>43</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>5000</v>
+      </c>
+      <c r="F13">
+        <v>357</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13" s="8">
+        <f t="shared" si="0"/>
+        <v>9.9824499999999997E-2</v>
+      </c>
+      <c r="I13" s="10">
+        <f t="shared" si="1"/>
+        <v>5.1073E-2</v>
+      </c>
+      <c r="N13" s="11">
+        <v>22</v>
+      </c>
+    </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+      <c r="C14">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>31</v>
+      </c>
+      <c r="E14">
+        <v>5000</v>
+      </c>
+      <c r="F14">
+        <v>346</v>
+      </c>
+      <c r="G14">
+        <v>4</v>
+      </c>
+      <c r="H14" s="8">
+        <f t="shared" si="0"/>
+        <v>2.3269999999999999E-2</v>
+      </c>
+      <c r="I14" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3992499999999994E-2</v>
+      </c>
+      <c r="N14" s="11">
+        <v>22</v>
+      </c>
       <c r="P14" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="2"/>
+        <v>595000</v>
+      </c>
+      <c r="C15">
+        <v>119</v>
+      </c>
+      <c r="D15">
+        <v>48</v>
+      </c>
+      <c r="E15">
+        <v>5000</v>
+      </c>
+      <c r="F15">
+        <v>357</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15" s="8">
+        <f t="shared" si="0"/>
+        <v>0.41438775</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="1"/>
+        <v>2.7857999999999997E-2</v>
+      </c>
+      <c r="N15" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="2"/>
+        <v>150000</v>
+      </c>
+      <c r="C16">
+        <v>30</v>
+      </c>
+      <c r="D16">
+        <v>24</v>
+      </c>
+      <c r="E16">
+        <v>5000</v>
+      </c>
+      <c r="F16">
+        <v>292</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16" s="8">
+        <f t="shared" si="0"/>
+        <v>8.8274999999999992E-2</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="1"/>
+        <v>6.4735000000000001E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="2"/>
+        <v>295000</v>
+      </c>
+      <c r="C17">
+        <v>59</v>
+      </c>
+      <c r="D17">
+        <v>20</v>
+      </c>
+      <c r="E17">
+        <v>5000</v>
+      </c>
+      <c r="F17">
+        <v>357</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17" s="8">
+        <f t="shared" si="0"/>
+        <v>0.17121062500000001</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3841250000000002E-2</v>
+      </c>
+      <c r="N17" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="2"/>
+        <v>155000</v>
+      </c>
+      <c r="C18">
+        <v>31</v>
+      </c>
+      <c r="D18">
+        <v>43</v>
+      </c>
+      <c r="E18">
+        <v>5000</v>
+      </c>
+      <c r="F18">
+        <v>357</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18" s="8">
+        <f t="shared" si="0"/>
+        <v>0.10794975</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="1"/>
+        <v>7.6609499999999997E-2</v>
+      </c>
+      <c r="N18" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="2"/>
+        <v>150000</v>
+      </c>
+      <c r="C19">
+        <v>30</v>
+      </c>
+      <c r="D19">
+        <v>11</v>
+      </c>
+      <c r="E19">
+        <v>5000</v>
+      </c>
+      <c r="F19">
+        <v>357</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19" s="8">
+        <f t="shared" si="0"/>
+        <v>6.9644999999999999E-2</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="1"/>
+        <v>5.1073E-2</v>
+      </c>
+      <c r="N19" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="2"/>
+        <v>175000</v>
+      </c>
+      <c r="C20">
+        <v>35</v>
+      </c>
+      <c r="D20">
+        <v>20</v>
+      </c>
+      <c r="E20">
+        <v>5000</v>
+      </c>
+      <c r="F20">
+        <v>357</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+      <c r="H20" s="8">
+        <f t="shared" si="0"/>
+        <v>0.10156562499999999</v>
+      </c>
+      <c r="I20" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3841250000000002E-2</v>
+      </c>
+      <c r="N20" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="2"/>
+        <v>60000</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>2546</v>
+      </c>
+      <c r="E21">
+        <v>5000</v>
+      </c>
+      <c r="F21">
+        <v>357</v>
+      </c>
+      <c r="G21">
+        <v>4</v>
+      </c>
+      <c r="H21" s="8">
+        <f t="shared" si="0"/>
+        <v>8.3573999999999996E-2</v>
+      </c>
+      <c r="I21" s="10">
+        <f t="shared" si="1"/>
+        <v>8.3573999999999996E-2</v>
+      </c>
+      <c r="N21" s="11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="2"/>
+        <v>165000</v>
+      </c>
+      <c r="C22">
+        <v>33</v>
+      </c>
+      <c r="D22">
+        <v>21</v>
+      </c>
+      <c r="E22">
+        <v>5000</v>
+      </c>
+      <c r="F22">
+        <v>357</v>
+      </c>
+      <c r="G22">
+        <v>4</v>
+      </c>
+      <c r="H22" s="8">
+        <f t="shared" si="0"/>
+        <v>9.5761874999999996E-2</v>
+      </c>
+      <c r="I22" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3841250000000002E-2</v>
+      </c>
+      <c r="N22" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="2"/>
+        <v>40000</v>
+      </c>
+      <c r="C23">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>400</v>
+      </c>
+      <c r="E23">
+        <v>5000</v>
+      </c>
+      <c r="F23">
+        <v>357</v>
+      </c>
+      <c r="G23">
+        <v>4</v>
+      </c>
+      <c r="H23" s="8">
+        <f t="shared" si="0"/>
+        <v>4.1786999999999998E-2</v>
+      </c>
+      <c r="I23" s="10">
+        <f t="shared" si="1"/>
+        <v>4.1786999999999998E-2</v>
+      </c>
+      <c r="N23" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="2"/>
+        <v>210000</v>
+      </c>
+      <c r="C24">
+        <v>42</v>
+      </c>
+      <c r="D24">
+        <v>27</v>
+      </c>
+      <c r="E24">
+        <v>5000</v>
+      </c>
+      <c r="F24">
+        <v>357</v>
+      </c>
+      <c r="G24">
+        <v>4</v>
+      </c>
+      <c r="H24" s="8">
+        <f t="shared" si="0"/>
+        <v>0.12187874999999999</v>
+      </c>
+      <c r="I24" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3841250000000002E-2</v>
+      </c>
+      <c r="N24" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="2"/>
+        <v>205000</v>
+      </c>
+      <c r="C25">
+        <v>41</v>
+      </c>
+      <c r="D25">
+        <v>32</v>
+      </c>
+      <c r="E25">
+        <v>5000</v>
+      </c>
+      <c r="F25">
+        <v>357</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+      <c r="H25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.118976875</v>
+      </c>
+      <c r="I25" s="10">
+        <f t="shared" si="1"/>
+        <v>6.3841250000000002E-2</v>
+      </c>
+      <c r="N25" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K27" s="8"/>
+    </row>
+    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C23" t="s">
+    <row r="34" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K34" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
+    <row r="35" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K35" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
+    <row r="36" spans="11:11" x14ac:dyDescent="0.2">
+      <c r="K36" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -7373,11 +9944,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5C8283-F952-754A-A544-78499AC1539F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+    <sheetView zoomScale="113" zoomScaleNormal="142" workbookViewId="0">
       <selection activeCell="V50" sqref="V50"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Spreadsheet now reflects the memory corrections; the memory of subseq is still theoretical but soon they will be confirmed with exerimental data
</commit_message>
<xml_diff>
--- a/final_experiments_data.xlsx
+++ b/final_experiments_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28221655-8406-7640-8DA9-10847F51E9A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75238FB8-B1DC-394E-87A6-8B02CF082717}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="20180" activeTab="7" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
+    <workbookView xWindow="51180" yWindow="460" windowWidth="38400" windowHeight="20180" activeTab="5" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy %" sheetId="1" r:id="rId1"/>
@@ -3178,25 +3178,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>3.0307212304728202</c:v>
+                  <c:v>1.5771206534022488</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3.0832080780051645</c:v>
+                  <c:v>1.3724822201045275</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8312225522532213</c:v>
+                  <c:v>1.2554092295724062</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5129574367834144</c:v>
+                  <c:v>1.9225867699045598</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.1024378737064504</c:v>
+                  <c:v>1.3335563156146075</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.722264720698895</c:v>
+                  <c:v>1.5370532526017042</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.3638985414746001</c:v>
+                  <c:v>1.5882248490024917</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8124,7 +8124,7 @@
   <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8175,7 +8175,8 @@
         <v>0.64</v>
       </c>
       <c r="F2" s="5">
-        <v>0.14000000000000001</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B2*LOG('Datasets Attributes, Notes'!D2,2) + 64 * 'Datasets Attributes, Notes'!D2 + 64)*0.000000125</f>
+        <v>7.2852920043018451E-2</v>
       </c>
       <c r="G2" s="8">
         <v>6.7000000000000004E-2</v>
@@ -8204,7 +8205,8 @@
         <v>0.77</v>
       </c>
       <c r="F3" s="5">
-        <v>0.22</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B3*LOG('Datasets Attributes, Notes'!D3,2) + 64 * 'Datasets Attributes, Notes'!D3 + 64)*0.000000125</f>
+        <v>9.7932439453893474E-2</v>
       </c>
       <c r="G3" s="8">
         <v>0.12</v>
@@ -8233,7 +8235,8 @@
         <v>0.17</v>
       </c>
       <c r="F4" s="5">
-        <v>0.2</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B4*LOG('Datasets Attributes, Notes'!D4,2) + 64 * 'Datasets Attributes, Notes'!D4 + 64)*0.000000125</f>
+        <v>4.305818268202808E-2</v>
       </c>
       <c r="G4" s="10">
         <v>2E-3</v>
@@ -8262,7 +8265,8 @@
         <v>1.95</v>
       </c>
       <c r="F5" s="5">
-        <v>0.12</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B5*LOG('Datasets Attributes, Notes'!D5,2) + 64 * 'Datasets Attributes, Notes'!D5 + 64)*0.000000125</f>
+        <v>9.1808324729867483E-2</v>
       </c>
       <c r="G5" s="8">
         <v>0.26</v>
@@ -8291,7 +8295,8 @@
         <v>0.21</v>
       </c>
       <c r="F6" s="5">
-        <v>0.15</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B6*LOG('Datasets Attributes, Notes'!D6,2) + 64 * 'Datasets Attributes, Notes'!D6 + 64)*0.000000125</f>
+        <v>4.8759653040514148E-2</v>
       </c>
       <c r="G6" s="8">
         <v>8.0000000000000002E-3</v>
@@ -8320,7 +8325,8 @@
         <v>106.14</v>
       </c>
       <c r="F7" s="5">
-        <v>2.25</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B7*LOG('Datasets Attributes, Notes'!D7,2) + 64 * 'Datasets Attributes, Notes'!D7 + 64)*0.000000125</f>
+        <v>2.0080361496056356</v>
       </c>
       <c r="G7" s="8">
         <v>26</v>
@@ -8349,7 +8355,8 @@
         <v>1.85</v>
       </c>
       <c r="F8" s="5">
-        <v>0.2</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B8*LOG('Datasets Attributes, Notes'!D8,2) + 64 * 'Datasets Attributes, Notes'!D8 + 64)*0.000000125</f>
+        <v>0.13437335157470481</v>
       </c>
       <c r="G8" s="8">
         <v>0.32</v>
@@ -8360,6 +8367,9 @@
       <c r="I8" s="8">
         <v>1</v>
       </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -8378,7 +8388,8 @@
         <v>0.1739</v>
       </c>
       <c r="F10" s="5">
-        <v>0.21460000000000001</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B10*LOG('Datasets Attributes, Notes'!D10,2) + 64 * 'Datasets Attributes, Notes'!D10 + 64)*0.000000125</f>
+        <v>2.2071624999999997E-2</v>
       </c>
       <c r="G10" s="8">
         <v>1.44E-4</v>
@@ -8407,7 +8418,8 @@
         <v>0.467084</v>
       </c>
       <c r="F11" s="5">
-        <v>0.64</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B11*LOG('Datasets Attributes, Notes'!D11,2) + 64 * 'Datasets Attributes, Notes'!D11 + 64)*0.000000125</f>
+        <v>0.16148585698521234</v>
       </c>
       <c r="G11" s="8">
         <v>3.2799999999999999E-3</v>
@@ -8436,7 +8448,8 @@
         <v>0.41660000000000003</v>
       </c>
       <c r="F12" s="5">
-        <v>0.65</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B12*LOG('Datasets Attributes, Notes'!D12,2) + 64 * 'Datasets Attributes, Notes'!D12 + 64)*0.000000125</f>
+        <v>0.12524267907741105</v>
       </c>
       <c r="G12" s="8">
         <v>8.4000000000000003E-4</v>
@@ -8465,7 +8478,8 @@
         <v>0.41899999999999998</v>
       </c>
       <c r="F13" s="5">
-        <v>0.65</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B13*LOG('Datasets Attributes, Notes'!D13,2) + 64 * 'Datasets Attributes, Notes'!D13 + 64)*0.000000125</f>
+        <v>0.1264740762980846</v>
       </c>
       <c r="G13" s="5">
         <v>1E-3</v>
@@ -8494,7 +8508,8 @@
         <v>0.25800000000000001</v>
       </c>
       <c r="F14" s="5">
-        <v>0.15</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B14*LOG('Datasets Attributes, Notes'!D14,2) + 64 * 'Datasets Attributes, Notes'!D14 + 64)*0.000000125</f>
+        <v>3.8654427415461677E-2</v>
       </c>
       <c r="G14" s="5">
         <v>4.0000000000000001E-3</v>
@@ -8523,7 +8538,8 @@
         <v>0.32700000000000001</v>
       </c>
       <c r="F15" s="5">
-        <v>1.7</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B15*LOG('Datasets Attributes, Notes'!D15,2) + 64 * 'Datasets Attributes, Notes'!D15 + 64)*0.000000125</f>
+        <v>0.58792307387273979</v>
       </c>
       <c r="G15" s="5">
         <v>6.0000000000000001E-3</v>
@@ -8552,7 +8568,8 @@
         <v>0.32</v>
       </c>
       <c r="F16" s="5">
-        <v>0.39</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B16*LOG('Datasets Attributes, Notes'!D16,2) + 64 * 'Datasets Attributes, Notes'!D16 + 64)*0.000000125</f>
+        <v>0.1002221031938572</v>
       </c>
       <c r="G16" s="9">
         <v>4.0000000000000001E-3</v>
@@ -8581,7 +8598,8 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="F17" s="5">
-        <v>0.9</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B17*LOG('Datasets Attributes, Notes'!D17,2) + 64 * 'Datasets Attributes, Notes'!D17 + 64)*0.000000125</f>
+        <v>0.22671509699831169</v>
       </c>
       <c r="G17" s="5">
         <v>3.0000000000000001E-3</v>
@@ -8610,7 +8628,8 @@
         <v>0.42</v>
       </c>
       <c r="F18" s="5">
-        <v>0.5</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B18*LOG('Datasets Attributes, Notes'!D18,2) + 64 * 'Datasets Attributes, Notes'!D18 + 64)*0.000000125</f>
+        <v>0.15477976436180282</v>
       </c>
       <c r="G18" s="5">
         <v>8.0000000000000002E-3</v>
@@ -8639,7 +8658,8 @@
         <v>0.22700000000000001</v>
       </c>
       <c r="F19" s="5">
-        <v>0.41</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B19*LOG('Datasets Attributes, Notes'!D19,2) + 64 * 'Datasets Attributes, Notes'!D19 + 64)*0.000000125</f>
+        <v>7.75784034639527E-2</v>
       </c>
       <c r="G19" s="5">
         <v>1E-3</v>
@@ -8667,8 +8687,9 @@
       <c r="E20" s="8">
         <v>0.253</v>
       </c>
-      <c r="F20" s="4">
-        <v>0.56000000000000005</v>
+      <c r="F20" s="5">
+        <f>(1.5*'Datasets Attributes, Notes'!B20*LOG('Datasets Attributes, Notes'!D20,2) + 64 * 'Datasets Attributes, Notes'!D20 + 64)*0.000000125</f>
+        <v>0.13753481196537029</v>
       </c>
       <c r="G20" s="5">
         <v>3.0000000000000001E-3</v>
@@ -8697,7 +8718,8 @@
         <v>1.792</v>
       </c>
       <c r="F21" s="5">
-        <v>0.22</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B21*LOG('Datasets Attributes, Notes'!D21,2) + 64 * 'Datasets Attributes, Notes'!D21 + 64)*0.000000125</f>
+        <v>0.14837335548998376</v>
       </c>
       <c r="G21" s="5">
         <v>0.123</v>
@@ -8726,7 +8748,8 @@
         <v>0.46400000000000002</v>
       </c>
       <c r="F22" s="5">
-        <v>0.52</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B22*LOG('Datasets Attributes, Notes'!D22,2) + 64 * 'Datasets Attributes, Notes'!D22 + 64)*0.000000125</f>
+        <v>0.13003074680687018</v>
       </c>
       <c r="G22" s="5">
         <v>4.0000000000000001E-3</v>
@@ -8755,7 +8778,8 @@
         <v>0.54100000000000004</v>
       </c>
       <c r="F23" s="5">
-        <v>0.15</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B23*LOG('Datasets Attributes, Notes'!D23,2) + 64 * 'Datasets Attributes, Notes'!D23 + 64)*0.000000125</f>
+        <v>7.2348117855238495E-2</v>
       </c>
       <c r="G23" s="5">
         <v>2.7E-2</v>
@@ -8784,7 +8808,8 @@
         <v>0.27400000000000002</v>
       </c>
       <c r="F24" s="5">
-        <v>0.65</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B24*LOG('Datasets Attributes, Notes'!D24,2) + 64 * 'Datasets Attributes, Notes'!D24 + 64)*0.000000125</f>
+        <v>0.17850286046471045</v>
       </c>
       <c r="G24" s="5">
         <v>5.0000000000000001E-3</v>
@@ -8813,7 +8838,8 @@
         <v>0.44400000000000001</v>
       </c>
       <c r="F25" s="5">
-        <v>0.64400000000000002</v>
+        <f>(1.5*'Datasets Attributes, Notes'!B25*LOG('Datasets Attributes, Notes'!D25,2) + 64 * 'Datasets Attributes, Notes'!D25 + 64)*0.000000125</f>
+        <v>0.18492243749999998</v>
       </c>
       <c r="G25" s="5">
         <v>7.0000000000000001E-3</v>
@@ -8835,8 +8861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA1A666-1255-6442-A7B1-7B11C7C732E9}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8894,7 +8920,7 @@
       </c>
       <c r="F2" s="8">
         <f>'Memory (MB)'!F2/'Datasets Attributes, Notes'!$H2</f>
-        <v>3.0307212304728202</v>
+        <v>1.5771206534022488</v>
       </c>
       <c r="G2" s="8">
         <f>'Memory (MB)'!G2/'Datasets Attributes, Notes'!$H2</f>
@@ -8931,7 +8957,7 @@
       </c>
       <c r="F3" s="8">
         <f>'Memory (MB)'!F3/'Datasets Attributes, Notes'!$H3</f>
-        <v>3.0832080780051645</v>
+        <v>1.3724822201045275</v>
       </c>
       <c r="G3" s="8">
         <f>'Memory (MB)'!G3/'Datasets Attributes, Notes'!$H3</f>
@@ -8968,7 +8994,7 @@
       </c>
       <c r="F4" s="8">
         <f>'Memory (MB)'!F4/'Datasets Attributes, Notes'!$H4</f>
-        <v>5.8312225522532213</v>
+        <v>1.2554092295724062</v>
       </c>
       <c r="G4" s="8">
         <f>'Memory (MB)'!G4/'Datasets Attributes, Notes'!$H4</f>
@@ -9005,7 +9031,7 @@
       </c>
       <c r="F5" s="8">
         <f>'Memory (MB)'!F5/'Datasets Attributes, Notes'!$H5</f>
-        <v>2.5129574367834144</v>
+        <v>1.9225867699045598</v>
       </c>
       <c r="G5" s="8">
         <f>'Memory (MB)'!G5/'Datasets Attributes, Notes'!$H5</f>
@@ -9042,7 +9068,7 @@
       </c>
       <c r="F6" s="8">
         <f>'Memory (MB)'!F6/'Datasets Attributes, Notes'!$H6</f>
-        <v>4.1024378737064504</v>
+        <v>1.3335563156146075</v>
       </c>
       <c r="G6" s="8">
         <f>'Memory (MB)'!G6/'Datasets Attributes, Notes'!$H6</f>
@@ -9079,7 +9105,7 @@
       </c>
       <c r="F7" s="8">
         <f>'Memory (MB)'!F7/'Datasets Attributes, Notes'!$H7</f>
-        <v>1.722264720698895</v>
+        <v>1.5370532526017042</v>
       </c>
       <c r="G7" s="8">
         <f>'Memory (MB)'!G7/'Datasets Attributes, Notes'!$H7</f>
@@ -9116,7 +9142,7 @@
       </c>
       <c r="F8" s="8">
         <f>'Memory (MB)'!F8/'Datasets Attributes, Notes'!$H8</f>
-        <v>2.3638985414746001</v>
+        <v>1.5882248490024917</v>
       </c>
       <c r="G8" s="8">
         <f>'Memory (MB)'!G8/'Datasets Attributes, Notes'!$H8</f>
@@ -9164,7 +9190,7 @@
       </c>
       <c r="F10" s="8">
         <f t="shared" si="0"/>
-        <v>1.3617465152194754</v>
+        <v>0.22226314180162302</v>
       </c>
       <c r="G10" s="8">
         <f t="shared" si="0"/>
@@ -9205,7 +9231,7 @@
       </c>
       <c r="F12" s="8">
         <f>'Memory (MB)'!F10/'Datasets Attributes, Notes'!$H10</f>
-        <v>14.610815135061532</v>
+        <v>1.502723357900291</v>
       </c>
       <c r="G12" s="8">
         <f>'Memory (MB)'!G10/'Datasets Attributes, Notes'!$H10</f>
@@ -9242,7 +9268,7 @@
       </c>
       <c r="F13" s="8">
         <f>'Memory (MB)'!F11/'Datasets Attributes, Notes'!$H11</f>
-        <v>5.1439450642741971</v>
+        <v>1.2979287140455811</v>
       </c>
       <c r="G13" s="8">
         <f>'Memory (MB)'!G11/'Datasets Attributes, Notes'!$H11</f>
@@ -9279,7 +9305,7 @@
       </c>
       <c r="F14" s="8">
         <f>'Memory (MB)'!F12/'Datasets Attributes, Notes'!$H12</f>
-        <v>6.4697539005150917</v>
+        <v>1.2465989407262155</v>
       </c>
       <c r="G14" s="8">
         <f>'Memory (MB)'!G12/'Datasets Attributes, Notes'!$H12</f>
@@ -9316,7 +9342,7 @@
       </c>
       <c r="F15" s="8">
         <f>'Memory (MB)'!F13/'Datasets Attributes, Notes'!$H13</f>
-        <v>6.4067181832518543</v>
+        <v>1.2465904066598783</v>
       </c>
       <c r="G15" s="8">
         <f>'Memory (MB)'!G13/'Datasets Attributes, Notes'!$H13</f>
@@ -9353,7 +9379,7 @@
       </c>
       <c r="F16" s="8">
         <f>'Memory (MB)'!F14/'Datasets Attributes, Notes'!$H14</f>
-        <v>5.8059365701429719</v>
+        <v>1.4961676915291069</v>
       </c>
       <c r="G16" s="8">
         <f>'Memory (MB)'!G14/'Datasets Attributes, Notes'!$H14</f>
@@ -9390,7 +9416,7 @@
       </c>
       <c r="F17" s="8">
         <f>'Memory (MB)'!F15/'Datasets Attributes, Notes'!$H15</f>
-        <v>4.0399719578417042</v>
+        <v>1.3971721951846856</v>
       </c>
       <c r="G17" s="8">
         <f>'Memory (MB)'!G15/'Datasets Attributes, Notes'!$H15</f>
@@ -9427,7 +9453,7 @@
       </c>
       <c r="F18" s="8">
         <f>'Memory (MB)'!F16/'Datasets Attributes, Notes'!$H16</f>
-        <v>5.3632206827792492</v>
+        <v>1.3782391197972594</v>
       </c>
       <c r="G18" s="8">
         <f>'Memory (MB)'!G16/'Datasets Attributes, Notes'!$H16</f>
@@ -9464,7 +9490,7 @@
       </c>
       <c r="F19" s="8">
         <f>'Memory (MB)'!F17/'Datasets Attributes, Notes'!$H17</f>
-        <v>5.1508962201721973</v>
+        <v>1.2975399290939742</v>
       </c>
       <c r="G19" s="8">
         <f>'Memory (MB)'!G17/'Datasets Attributes, Notes'!$H17</f>
@@ -9501,7 +9527,7 @@
       </c>
       <c r="F20" s="8">
         <f>'Memory (MB)'!F18/'Datasets Attributes, Notes'!$H18</f>
-        <v>4.3922354062488331</v>
+        <v>1.3596583224015235</v>
       </c>
       <c r="G20" s="8">
         <f>'Memory (MB)'!G18/'Datasets Attributes, Notes'!$H18</f>
@@ -9538,7 +9564,7 @@
       </c>
       <c r="F21" s="8">
         <f>'Memory (MB)'!F19/'Datasets Attributes, Notes'!$H19</f>
-        <v>6.8646245803788943</v>
+        <v>1.2988941837200021</v>
       </c>
       <c r="G21" s="8">
         <f>'Memory (MB)'!G19/'Datasets Attributes, Notes'!$H19</f>
@@ -9575,7 +9601,7 @@
       </c>
       <c r="F22" s="8">
         <f>'Memory (MB)'!F20/'Datasets Attributes, Notes'!$H20</f>
-        <v>5.2857302979712477</v>
+        <v>1.2981641475556003</v>
       </c>
       <c r="G22" s="8">
         <f>'Memory (MB)'!G20/'Datasets Attributes, Notes'!$H20</f>
@@ -9612,7 +9638,7 @@
       </c>
       <c r="F23" s="8">
         <f>'Memory (MB)'!F21/'Datasets Attributes, Notes'!$H21</f>
-        <v>2.4113288614143542</v>
+        <v>1.6262588834449534</v>
       </c>
       <c r="G23" s="8">
         <f>'Memory (MB)'!G21/'Datasets Attributes, Notes'!$H21</f>
@@ -9649,7 +9675,7 @@
       </c>
       <c r="F24" s="8">
         <f>'Memory (MB)'!F22/'Datasets Attributes, Notes'!$H22</f>
-        <v>5.2766767084192177</v>
+        <v>1.3194811789503238</v>
       </c>
       <c r="G24" s="8">
         <f>'Memory (MB)'!G22/'Datasets Attributes, Notes'!$H22</f>
@@ -9686,7 +9712,7 @@
       </c>
       <c r="F25" s="8">
         <f>'Memory (MB)'!F23/'Datasets Attributes, Notes'!$H23</f>
-        <v>3.1120654778576542</v>
+        <v>1.5010138664350978</v>
       </c>
       <c r="G25" s="8">
         <f>'Memory (MB)'!G23/'Datasets Attributes, Notes'!$H23</f>
@@ -9723,7 +9749,7 @@
       </c>
       <c r="F26" s="8">
         <f>'Memory (MB)'!F24/'Datasets Attributes, Notes'!$H24</f>
-        <v>5.2008581415933639</v>
+        <v>1.4282585463778361</v>
       </c>
       <c r="G26" s="8">
         <f>'Memory (MB)'!G24/'Datasets Attributes, Notes'!$H24</f>
@@ -9760,7 +9786,7 @@
       </c>
       <c r="F27" s="8">
         <f>'Memory (MB)'!F25/'Datasets Attributes, Notes'!$H25</f>
-        <v>5.2312800491447895</v>
+        <v>1.5021444998959226</v>
       </c>
       <c r="G27" s="8">
         <f>'Memory (MB)'!G25/'Datasets Attributes, Notes'!$H25</f>
@@ -9786,7 +9812,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10574,7 +10600,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E5C8283-F952-754A-A544-78499AC1539F}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="142" workbookViewId="0">
+    <sheetView topLeftCell="E1" zoomScale="125" zoomScaleNormal="142" workbookViewId="0">
       <selection activeCell="O62" sqref="O62"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
exported results so far, after all the changes
</commit_message>
<xml_diff>
--- a/final_experiments_data.xlsx
+++ b/final_experiments_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75238FB8-B1DC-394E-87A6-8B02CF082717}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33895433-C293-9544-B3D9-81CE51BA99DD}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51180" yWindow="460" windowWidth="38400" windowHeight="20180" activeTab="5" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="20100" activeTab="1" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy %" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="56">
   <si>
     <t>DG</t>
   </si>
@@ -183,6 +183,24 @@
   <si>
     <t>St. Deviation</t>
   </si>
+  <si>
+    <t>#ranks</t>
+  </si>
+  <si>
+    <t>#L[]</t>
+  </si>
+  <si>
+    <t>#sdsl::wt::interval_scans</t>
+  </si>
+  <si>
+    <t>% ranks</t>
+  </si>
+  <si>
+    <t>% L[]</t>
+  </si>
+  <si>
+    <t>%s cans</t>
+  </si>
 </sst>
 </file>
 
@@ -245,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -265,6 +283,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2009,25 +2028,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>1729.1066282420747</c:v>
+                  <c:v>443.17002881844383</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8076.9230769230762</c:v>
+                  <c:v>2324.0384615384614</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>330.53221288515408</c:v>
+                  <c:v>61.400560224089645</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>965.90909090909099</c:v>
+                  <c:v>290.76704545454544</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>243.69747899159663</c:v>
+                  <c:v>48.011204481792717</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30214.68574984443</c:v>
+                  <c:v>14939.016801493466</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3352.1126760563379</c:v>
+                  <c:v>960.95774647887322</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7453,10 +7472,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D61A1C-C42B-6442-B132-77D4B94522A1}">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7464,7 +7483,7 @@
     <col min="10" max="10" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="2"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -7493,8 +7512,26 @@
       <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -7516,7 +7553,7 @@
       </c>
       <c r="F2" s="8">
         <f>'Exec. Time of Test Phase (ms)'!F2/'Datasets Attributes, Notes'!$F2*1000</f>
-        <v>1729.1066282420747</v>
+        <v>443.17002881844383</v>
       </c>
       <c r="G2" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G2/'Datasets Attributes, Notes'!$F2*1000</f>
@@ -7534,8 +7571,32 @@
         <f>'Exec. Time of Test Phase (ms)'!J2/'Datasets Attributes, Notes'!$F2*1000</f>
         <v>1068884.7262247838</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M2" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!L2/'Datasets Attributes, Notes'!$F2</f>
+        <v>2408.1543845203787</v>
+      </c>
+      <c r="N2" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!M2/'Datasets Attributes, Notes'!$F2</f>
+        <v>278.87813915191435</v>
+      </c>
+      <c r="O2" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!N2/'Datasets Attributes, Notes'!$F2</f>
+        <v>49.114244545080282</v>
+      </c>
+      <c r="Q2" s="15">
+        <f>M2/SUM(M2:O2)</f>
+        <v>0.88012617323496689</v>
+      </c>
+      <c r="R2" s="15">
+        <f>N2/SUM(M2:O2)</f>
+        <v>0.10192367689895751</v>
+      </c>
+      <c r="S2" s="15">
+        <f>O2/SUM(M2:O2)</f>
+        <v>1.7950149866075606E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -7557,7 +7618,7 @@
       </c>
       <c r="F3" s="8">
         <f>'Exec. Time of Test Phase (ms)'!F3/'Datasets Attributes, Notes'!$F3*1000</f>
-        <v>8076.9230769230762</v>
+        <v>2324.0384615384614</v>
       </c>
       <c r="G3" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G3/'Datasets Attributes, Notes'!$F3*1000</f>
@@ -7575,8 +7636,32 @@
         <f>'Exec. Time of Test Phase (ms)'!J3/'Datasets Attributes, Notes'!$F3*1000</f>
         <v>6730.7692307692305</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M3" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!L3/'Datasets Attributes, Notes'!$F3</f>
+        <v>13803.506868131868</v>
+      </c>
+      <c r="N3" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!M3/'Datasets Attributes, Notes'!$F3</f>
+        <v>2489.348901098901</v>
+      </c>
+      <c r="O3" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!N3/'Datasets Attributes, Notes'!$F3</f>
+        <v>358.74862637362639</v>
+      </c>
+      <c r="Q3" s="15">
+        <f t="shared" ref="Q3:Q8" si="0">M3/SUM(M3:O3)</f>
+        <v>0.8289595729151269</v>
+      </c>
+      <c r="R3" s="15">
+        <f t="shared" ref="R3:R8" si="1">N3/SUM(M3:O3)</f>
+        <v>0.14949603905771547</v>
+      </c>
+      <c r="S3" s="15">
+        <f t="shared" ref="S3:S8" si="2">O3/SUM(M3:O3)</f>
+        <v>2.1544388027157732E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -7598,7 +7683,7 @@
       </c>
       <c r="F4" s="8">
         <f>'Exec. Time of Test Phase (ms)'!F4/'Datasets Attributes, Notes'!$F4*1000</f>
-        <v>330.53221288515408</v>
+        <v>61.400560224089645</v>
       </c>
       <c r="G4" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G4/'Datasets Attributes, Notes'!$F4*1000</f>
@@ -7616,8 +7701,32 @@
         <f>'Exec. Time of Test Phase (ms)'!J4/'Datasets Attributes, Notes'!$F4*1000</f>
         <v>308.12324929971993</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M4" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!L4/'Datasets Attributes, Notes'!$F4</f>
+        <v>332.81452581032414</v>
+      </c>
+      <c r="N4" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!M4/'Datasets Attributes, Notes'!$F4</f>
+        <v>522.69027611044419</v>
+      </c>
+      <c r="O4" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!N4/'Datasets Attributes, Notes'!$F4</f>
+        <v>2.8877551020408161</v>
+      </c>
+      <c r="Q4" s="15">
+        <f t="shared" si="0"/>
+        <v>0.38771832664140932</v>
+      </c>
+      <c r="R4" s="15">
+        <f t="shared" si="1"/>
+        <v>0.60891753060314013</v>
+      </c>
+      <c r="S4" s="15">
+        <f t="shared" si="2"/>
+        <v>3.3641427554503859E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -7639,7 +7748,7 @@
       </c>
       <c r="F5" s="8">
         <f>'Exec. Time of Test Phase (ms)'!F5/'Datasets Attributes, Notes'!$F5*1000</f>
-        <v>965.90909090909099</v>
+        <v>290.76704545454544</v>
       </c>
       <c r="G5" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G5/'Datasets Attributes, Notes'!$F5*1000</f>
@@ -7657,8 +7766,32 @@
         <f>'Exec. Time of Test Phase (ms)'!J5/'Datasets Attributes, Notes'!$F5*1000</f>
         <v>75000</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M5" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!L5/'Datasets Attributes, Notes'!$F5</f>
+        <v>854.30864448051943</v>
+      </c>
+      <c r="N5" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!M5/'Datasets Attributes, Notes'!$F5</f>
+        <v>949.28814935064941</v>
+      </c>
+      <c r="O5" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!N5/'Datasets Attributes, Notes'!$F5</f>
+        <v>3.859375</v>
+      </c>
+      <c r="Q5" s="15">
+        <f t="shared" si="0"/>
+        <v>0.47265801473513847</v>
+      </c>
+      <c r="R5" s="15">
+        <f t="shared" si="1"/>
+        <v>0.52520673293257647</v>
+      </c>
+      <c r="S5" s="15">
+        <f t="shared" si="2"/>
+        <v>2.1352523322851862E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -7680,7 +7813,7 @@
       </c>
       <c r="F6" s="8">
         <f>'Exec. Time of Test Phase (ms)'!F6/'Datasets Attributes, Notes'!$F6*1000</f>
-        <v>243.69747899159663</v>
+        <v>48.011204481792717</v>
       </c>
       <c r="G6" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G6/'Datasets Attributes, Notes'!$F6*1000</f>
@@ -7698,8 +7831,32 @@
         <f>'Exec. Time of Test Phase (ms)'!J6/'Datasets Attributes, Notes'!$F6*1000</f>
         <v>2156.8627450980389</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M6" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!L6/'Datasets Attributes, Notes'!$F6</f>
+        <v>274.90376150460185</v>
+      </c>
+      <c r="N6" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!M6/'Datasets Attributes, Notes'!$F6</f>
+        <v>339.90596238495397</v>
+      </c>
+      <c r="O6" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!N6/'Datasets Attributes, Notes'!$F6</f>
+        <v>3.4773909563825529</v>
+      </c>
+      <c r="Q6" s="15">
+        <f t="shared" si="0"/>
+        <v>0.44462152761035778</v>
+      </c>
+      <c r="R6" s="15">
+        <f t="shared" si="1"/>
+        <v>0.54975423912828913</v>
+      </c>
+      <c r="S6" s="15">
+        <f t="shared" si="2"/>
+        <v>5.6242332613530713E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -7721,7 +7878,7 @@
       </c>
       <c r="F7" s="8">
         <f>'Exec. Time of Test Phase (ms)'!F7/'Datasets Attributes, Notes'!$F7*1000</f>
-        <v>30214.68574984443</v>
+        <v>14939.016801493466</v>
       </c>
       <c r="G7" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G7/'Datasets Attributes, Notes'!$F7*1000</f>
@@ -7739,8 +7896,32 @@
         <f>'Exec. Time of Test Phase (ms)'!J7/'Datasets Attributes, Notes'!$F7*1000</f>
         <v>619985.37647790916</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M7" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!L7/'Datasets Attributes, Notes'!$F7</f>
+        <v>32807.102609120811</v>
+      </c>
+      <c r="N7" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!M7/'Datasets Attributes, Notes'!$F7</f>
+        <v>618.10516490354701</v>
+      </c>
+      <c r="O7" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!N7/'Datasets Attributes, Notes'!$F7</f>
+        <v>477.65174682193975</v>
+      </c>
+      <c r="Q7" s="15">
+        <f t="shared" si="0"/>
+        <v>0.96767951355101123</v>
+      </c>
+      <c r="R7" s="15">
+        <f t="shared" si="1"/>
+        <v>1.8231652835168213E-2</v>
+      </c>
+      <c r="S7" s="15">
+        <f t="shared" si="2"/>
+        <v>1.408883361382068E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -7762,7 +7943,7 @@
       </c>
       <c r="F8" s="8">
         <f>'Exec. Time of Test Phase (ms)'!F8/'Datasets Attributes, Notes'!$F8*1000</f>
-        <v>3352.1126760563379</v>
+        <v>960.95774647887322</v>
       </c>
       <c r="G8" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G8/'Datasets Attributes, Notes'!$F8*1000</f>
@@ -7780,8 +7961,32 @@
         <f>'Exec. Time of Test Phase (ms)'!J8/'Datasets Attributes, Notes'!$F8*1000</f>
         <v>51107.042253521133</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="M8" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!L8/'Datasets Attributes, Notes'!$F8</f>
+        <v>4383.1907444668013</v>
+      </c>
+      <c r="N8" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!M8/'Datasets Attributes, Notes'!$F8</f>
+        <v>1120.2812877263582</v>
+      </c>
+      <c r="O8" s="3">
+        <f>'Exec. Time of Test Phase (ms)'!N8/'Datasets Attributes, Notes'!$F8</f>
+        <v>61.060160965794765</v>
+      </c>
+      <c r="Q8" s="15">
+        <f t="shared" si="0"/>
+        <v>0.78770156992810703</v>
+      </c>
+      <c r="R8" s="15">
+        <f t="shared" si="1"/>
+        <v>0.20132533137352207</v>
+      </c>
+      <c r="S8" s="15">
+        <f t="shared" si="2"/>
+        <v>1.0973098698370768E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>49</v>
       </c>
@@ -7790,35 +7995,35 @@
         <v>3.6281778267268345</v>
       </c>
       <c r="C11">
-        <f t="shared" ref="C11:J11" si="0">STDEV(C2:C8)</f>
+        <f t="shared" ref="C11:J11" si="3">STDEV(C2:C8)</f>
         <v>0.42383683374854919</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>634.52898411372792</v>
       </c>
       <c r="E11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>676.36590599325609</v>
       </c>
       <c r="F11">
-        <f t="shared" si="0"/>
-        <v>10842.233866398023</v>
+        <f t="shared" si="3"/>
+        <v>5444.3867484700904</v>
       </c>
       <c r="G11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.7537068164296357</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>2.3512921176947099</v>
       </c>
       <c r="I11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>45.256040268102595</v>
       </c>
       <c r="J11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>420279.86892522278</v>
       </c>
     </row>
@@ -7829,18 +8034,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BA0485-4631-4D4D-BD6C-8B9119B36FE5}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:N8"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="51" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7868,8 +8075,17 @@
       <c r="J1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -7885,8 +8101,8 @@
       <c r="E2" s="8">
         <v>96.6</v>
       </c>
-      <c r="F2" s="4">
-        <v>600</v>
+      <c r="F2" s="3">
+        <v>153.78</v>
       </c>
       <c r="G2" s="8">
         <v>0.35</v>
@@ -7900,8 +8116,17 @@
       <c r="J2" s="4">
         <v>370903</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L2" s="3">
+        <v>835629.57142857148</v>
+      </c>
+      <c r="M2" s="3">
+        <v>96770.71428571429</v>
+      </c>
+      <c r="N2" s="3">
+        <v>17042.642857142859</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -7918,7 +8143,7 @@
         <v>41.21</v>
       </c>
       <c r="F3" s="4">
-        <v>420</v>
+        <v>120.85</v>
       </c>
       <c r="G3" s="8">
         <v>0.28000000000000003</v>
@@ -7932,8 +8157,17 @@
       <c r="J3" s="4">
         <v>350</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L3" s="3">
+        <v>717782.35714285716</v>
+      </c>
+      <c r="M3" s="3">
+        <v>129446.14285714286</v>
+      </c>
+      <c r="N3" s="3">
+        <v>18654.928571428572</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -7950,7 +8184,7 @@
         <v>24.14</v>
       </c>
       <c r="F4" s="4">
-        <v>118</v>
+        <v>21.92</v>
       </c>
       <c r="G4" s="8">
         <v>0</v>
@@ -7964,8 +8198,17 @@
       <c r="J4" s="4">
         <v>110</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L4" s="3">
+        <v>118814.78571428571</v>
+      </c>
+      <c r="M4" s="3">
+        <v>186600.42857142858</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1030.9285714285713</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -7982,7 +8225,7 @@
         <v>7.07</v>
       </c>
       <c r="F5" s="4">
-        <v>340</v>
+        <v>102.35</v>
       </c>
       <c r="G5" s="8">
         <v>1.07</v>
@@ -7996,8 +8239,17 @@
       <c r="J5" s="4">
         <v>26400</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L5" s="3">
+        <v>300716.64285714284</v>
+      </c>
+      <c r="M5" s="3">
+        <v>334149.42857142858</v>
+      </c>
+      <c r="N5" s="3">
+        <v>1358.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -8014,7 +8266,7 @@
         <v>7.35</v>
       </c>
       <c r="F6" s="4">
-        <v>87</v>
+        <v>17.14</v>
       </c>
       <c r="G6" s="8">
         <v>0.14000000000000001</v>
@@ -8028,8 +8280,17 @@
       <c r="J6" s="4">
         <v>770</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L6" s="3">
+        <v>98140.642857142855</v>
+      </c>
+      <c r="M6" s="3">
+        <v>121346.42857142857</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1241.4285714285713</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -8045,8 +8306,8 @@
       <c r="E7" s="8">
         <v>5897</v>
       </c>
-      <c r="F7" s="5">
-        <v>97110</v>
+      <c r="F7" s="4">
+        <v>48014</v>
       </c>
       <c r="G7" s="8">
         <v>23.92</v>
@@ -8060,8 +8321,17 @@
       <c r="J7" s="4">
         <v>1992633</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="L7" s="3">
+        <v>105442027.78571428</v>
+      </c>
+      <c r="M7" s="3">
+        <v>1986590</v>
+      </c>
+      <c r="N7" s="3">
+        <v>1535172.7142857143</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -8077,8 +8347,8 @@
       <c r="E8" s="8">
         <v>15</v>
       </c>
-      <c r="F8" s="9">
-        <v>1190</v>
+      <c r="F8" s="4">
+        <v>341.14</v>
       </c>
       <c r="G8" s="8">
         <v>0.78</v>
@@ -8091,6 +8361,15 @@
       </c>
       <c r="J8" s="4">
         <v>18143</v>
+      </c>
+      <c r="L8" s="3">
+        <v>1556032.7142857143</v>
+      </c>
+      <c r="M8" s="3">
+        <v>397699.85714285716</v>
+      </c>
+      <c r="N8" s="3">
+        <v>21676.357142857141</v>
       </c>
     </row>
   </sheetData>
@@ -8121,10 +8400,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9058626D-1839-5446-B7A4-B72B5F5525AF}">
-  <dimension ref="A1:I25"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8132,7 +8411,7 @@
     <col min="1" max="1" width="27.6640625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8158,7 +8437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -8188,7 +8467,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -8218,7 +8497,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
@@ -8248,7 +8527,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
@@ -8278,7 +8557,7 @@
         <v>0.52</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
@@ -8308,7 +8587,7 @@
         <v>1.39</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -8337,8 +8616,9 @@
       <c r="I7" s="8">
         <v>5.97</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
@@ -8368,10 +8648,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>31</v>
       </c>
@@ -8401,7 +8681,7 @@
         <v>8.3239999999999995E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>32</v>
       </c>
@@ -8431,7 +8711,7 @@
         <v>0.72475000000000001</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>33</v>
       </c>
@@ -8461,7 +8741,7 @@
         <v>0.59789999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>34</v>
       </c>
@@ -8491,7 +8771,7 @@
         <v>0.61299999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>35</v>
       </c>
@@ -8521,7 +8801,7 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -8551,7 +8831,7 @@
         <v>1.385</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>37</v>
       </c>
@@ -8861,8 +9141,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA1A666-1255-6442-A7B1-7B11C7C732E9}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9812,7 +10092,7 @@
   <dimension ref="A1:O36"/>
   <sheetViews>
     <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added some latest data; one of them is the updated running times without the sub-patters ??abc predicionts. Also included running times for the predictor with a direct access to BWT uint64_t*
</commit_message>
<xml_diff>
--- a/final_experiments_data.xlsx
+++ b/final_experiments_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C9DFBA-58BC-6C48-9581-B76833718834}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D34A6A-E49B-F74C-8B0F-777C25A1F6C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="20100" activeTab="1" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
+    <workbookView xWindow="51200" yWindow="460" windowWidth="38400" windowHeight="20100" activeTab="2" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy %" sheetId="1" r:id="rId1"/>
@@ -2073,25 +2073,25 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>438.04034582132567</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2324.0384615384614</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>61.400560224089645</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>290.76704545454544</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>48.011204481792717</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14939.016801493466</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>957.74647887323943</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7519,7 +7519,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74D61A1C-C42B-6442-B132-77D4B94522A1}">
   <dimension ref="A1:S11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
@@ -7596,9 +7596,9 @@
         <f>'Exec. Time of Test Phase (ms)'!E2/'Datasets Attributes, Notes'!$F2*1000</f>
         <v>278.38616714697406</v>
       </c>
-      <c r="F2" s="8">
-        <f>'Exec. Time of Test Phase (ms)'!F2/'Datasets Attributes, Notes'!$F2*1000</f>
-        <v>438.04034582132567</v>
+      <c r="F2" s="8" t="e">
+        <f>'Exec. Time of Test Phase (ms)'!#REF!/'Datasets Attributes, Notes'!$F2*1000</f>
+        <v>#REF!</v>
       </c>
       <c r="G2" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G2/'Datasets Attributes, Notes'!$F2*1000</f>
@@ -7661,9 +7661,9 @@
         <f>'Exec. Time of Test Phase (ms)'!E3/'Datasets Attributes, Notes'!$F3*1000</f>
         <v>792.5</v>
       </c>
-      <c r="F3" s="8">
-        <f>'Exec. Time of Test Phase (ms)'!F3/'Datasets Attributes, Notes'!$F3*1000</f>
-        <v>2324.0384615384614</v>
+      <c r="F3" s="8" t="e">
+        <f>'Exec. Time of Test Phase (ms)'!#REF!/'Datasets Attributes, Notes'!$F3*1000</f>
+        <v>#REF!</v>
       </c>
       <c r="G3" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G3/'Datasets Attributes, Notes'!$F3*1000</f>
@@ -7726,9 +7726,9 @@
         <f>'Exec. Time of Test Phase (ms)'!E4/'Datasets Attributes, Notes'!$F4*1000</f>
         <v>67.61904761904762</v>
       </c>
-      <c r="F4" s="8">
-        <f>'Exec. Time of Test Phase (ms)'!F4/'Datasets Attributes, Notes'!$F4*1000</f>
-        <v>61.400560224089645</v>
+      <c r="F4" s="8" t="e">
+        <f>'Exec. Time of Test Phase (ms)'!#REF!/'Datasets Attributes, Notes'!$F4*1000</f>
+        <v>#REF!</v>
       </c>
       <c r="G4" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G4/'Datasets Attributes, Notes'!$F4*1000</f>
@@ -7791,9 +7791,9 @@
         <f>'Exec. Time of Test Phase (ms)'!E5/'Datasets Attributes, Notes'!$F5*1000</f>
         <v>20.085227272727273</v>
       </c>
-      <c r="F5" s="8">
-        <f>'Exec. Time of Test Phase (ms)'!F5/'Datasets Attributes, Notes'!$F5*1000</f>
-        <v>290.76704545454544</v>
+      <c r="F5" s="8" t="e">
+        <f>'Exec. Time of Test Phase (ms)'!#REF!/'Datasets Attributes, Notes'!$F5*1000</f>
+        <v>#REF!</v>
       </c>
       <c r="G5" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G5/'Datasets Attributes, Notes'!$F5*1000</f>
@@ -7856,9 +7856,9 @@
         <f>'Exec. Time of Test Phase (ms)'!E6/'Datasets Attributes, Notes'!$F6*1000</f>
         <v>20.588235294117649</v>
       </c>
-      <c r="F6" s="8">
-        <f>'Exec. Time of Test Phase (ms)'!F6/'Datasets Attributes, Notes'!$F6*1000</f>
-        <v>48.011204481792717</v>
+      <c r="F6" s="8" t="e">
+        <f>'Exec. Time of Test Phase (ms)'!#REF!/'Datasets Attributes, Notes'!$F6*1000</f>
+        <v>#REF!</v>
       </c>
       <c r="G6" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G6/'Datasets Attributes, Notes'!$F6*1000</f>
@@ -7921,9 +7921,9 @@
         <f>'Exec. Time of Test Phase (ms)'!E7/'Datasets Attributes, Notes'!$F7*1000</f>
         <v>1834.7853142501556</v>
       </c>
-      <c r="F7" s="8">
-        <f>'Exec. Time of Test Phase (ms)'!F7/'Datasets Attributes, Notes'!$F7*1000</f>
-        <v>14939.016801493466</v>
+      <c r="F7" s="8" t="e">
+        <f>'Exec. Time of Test Phase (ms)'!#REF!/'Datasets Attributes, Notes'!$F7*1000</f>
+        <v>#REF!</v>
       </c>
       <c r="G7" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G7/'Datasets Attributes, Notes'!$F7*1000</f>
@@ -7986,9 +7986,9 @@
         <f>'Exec. Time of Test Phase (ms)'!E8/'Datasets Attributes, Notes'!$F8*1000</f>
         <v>42.25352112676056</v>
       </c>
-      <c r="F8" s="8">
-        <f>'Exec. Time of Test Phase (ms)'!F8/'Datasets Attributes, Notes'!$F8*1000</f>
-        <v>957.74647887323943</v>
+      <c r="F8" s="8" t="e">
+        <f>'Exec. Time of Test Phase (ms)'!#REF!/'Datasets Attributes, Notes'!$F8*1000</f>
+        <v>#REF!</v>
       </c>
       <c r="G8" s="8">
         <f>'Exec. Time of Test Phase (ms)'!G8/'Datasets Attributes, Notes'!$F8*1000</f>
@@ -8051,9 +8051,9 @@
         <f t="shared" si="3"/>
         <v>676.36590599325609</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="e">
         <f t="shared" si="3"/>
-        <v>5444.9185888956445</v>
+        <v>#REF!</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
@@ -8081,8 +8081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7BA0485-4631-4D4D-BD6C-8B9119B36FE5}">
   <dimension ref="A1:N8"/>
   <sheetViews>
-    <sheetView zoomScale="142" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView tabSelected="1" zoomScale="142" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8147,7 +8147,7 @@
         <v>96.6</v>
       </c>
       <c r="F2" s="3">
-        <v>152</v>
+        <v>81</v>
       </c>
       <c r="G2" s="8">
         <v>0.35</v>
@@ -8187,8 +8187,8 @@
       <c r="E3" s="8">
         <v>41.21</v>
       </c>
-      <c r="F3" s="4">
-        <v>120.85</v>
+      <c r="F3" s="3">
+        <v>117</v>
       </c>
       <c r="G3" s="8">
         <v>0.28000000000000003</v>
@@ -8228,8 +8228,8 @@
       <c r="E4" s="8">
         <v>24.14</v>
       </c>
-      <c r="F4" s="4">
-        <v>21.92</v>
+      <c r="F4" s="3">
+        <v>21</v>
       </c>
       <c r="G4" s="8">
         <v>0</v>
@@ -8269,8 +8269,8 @@
       <c r="E5" s="8">
         <v>7.07</v>
       </c>
-      <c r="F5" s="4">
-        <v>102.35</v>
+      <c r="F5" s="3">
+        <v>94</v>
       </c>
       <c r="G5" s="8">
         <v>1.07</v>
@@ -8310,8 +8310,8 @@
       <c r="E6" s="8">
         <v>7.35</v>
       </c>
-      <c r="F6" s="4">
-        <v>17.14</v>
+      <c r="F6" s="3">
+        <v>16</v>
       </c>
       <c r="G6" s="8">
         <v>0.14000000000000001</v>
@@ -8351,8 +8351,8 @@
       <c r="E7" s="8">
         <v>5897</v>
       </c>
-      <c r="F7" s="4">
-        <v>48014</v>
+      <c r="F7" s="3">
+        <v>33089</v>
       </c>
       <c r="G7" s="8">
         <v>23.92</v>
@@ -8392,8 +8392,8 @@
       <c r="E8" s="8">
         <v>15</v>
       </c>
-      <c r="F8" s="4">
-        <v>340</v>
+      <c r="F8" s="3">
+        <v>177</v>
       </c>
       <c r="G8" s="8">
         <v>0.78</v>

</xml_diff>

<commit_message>
made scalability charts presentation more consistent
</commit_message>
<xml_diff>
--- a/final_experiments_data.xlsx
+++ b/final_experiments_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rafaelktistakis/Repositories/sBP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEEA29DF-7596-4642-AB83-537D61538B0F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F204A90F-46A6-5644-8679-069D368812FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51200" windowHeight="28800" activeTab="8" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
+    <workbookView xWindow="51200" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="8" xr2:uid="{B8C33F8D-BADD-D24B-82DA-2EDA7EEB5B99}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy %" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,6 @@
     <sheet name="Scalability Charts" sheetId="10" r:id="rId9"/>
     <sheet name="Performance Charts" sheetId="5" r:id="rId10"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Scalability CPT+'!$B$1:$G$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Scalability CPT+'!$B$2:$G$2</definedName>
-  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -828,6 +824,7 @@
       <c:valAx>
         <c:axId val="1435843999"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -1439,7 +1436,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5410,7 +5407,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -5984,7 +5981,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -6226,16 +6223,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6247,16 +6244,16 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1616.71</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3179.241</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4421.4040000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1882.4839999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4421.4040000000005</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3179.241</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1616.71</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6305,16 +6302,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6326,16 +6323,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>4.2885</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.1141300000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.2238699999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>4.3745700000000003</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.2238699999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>4.1141300000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4.2885</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6469,6 +6466,7 @@
       <c:valAx>
         <c:axId val="1435843999"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6792,16 +6790,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6813,16 +6811,16 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>0.96599999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.78500000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3879999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>1.4510000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1.3879999999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.78500000000000003</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.96599999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6871,16 +6869,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6892,16 +6890,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>1.0930200000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.73525399999999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.36714999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>7.2503999999999999E-2</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.36714999999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.73525399999999996</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1.0930200000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7113,7 +7111,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -7363,16 +7361,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7384,16 +7382,16 @@
                 <c:formatCode>0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>20.472999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>40.835000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75.563999999999993</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>110.43899999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75.563999999999993</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>40.835000000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>20.472999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7442,16 +7440,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>12</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7463,16 +7461,16 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>6.96333</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.07735</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.2179900000000004</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>6.6927099999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>7.2179900000000004</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>7.07735</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>6.96333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8137,7 +8135,7 @@
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -8181,6 +8179,7 @@
       <c:valAx>
         <c:axId val="1435843999"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -8824,7 +8823,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -21831,8 +21830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C2CA90-8492-FA44-8F31-E345E5B9D4A9}">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41"/>
+    <sheetView topLeftCell="A11" zoomScale="142" zoomScaleNormal="142" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22757,19 +22756,19 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B34">
-        <v>3733343</v>
+        <v>3918478</v>
       </c>
       <c r="C34">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D34">
-        <v>908</v>
+        <v>915</v>
       </c>
       <c r="E34">
-        <v>872472</v>
+        <v>150000</v>
       </c>
       <c r="F34">
         <v>100</v>
@@ -22778,25 +22777,25 @@
         <v>4</v>
       </c>
       <c r="H34" s="18">
-        <f t="shared" si="1"/>
-        <v>4.66667875</v>
+        <f t="shared" ref="H34" si="2">(_xlfn.CEILING.MATH(LOG(D34, 2)))*(B34)*0.000000125</f>
+        <v>4.8980974999999995</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B35">
-        <v>4036428</v>
+        <v>3983033</v>
       </c>
       <c r="C35">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D35">
         <v>912</v>
       </c>
       <c r="E35">
-        <v>567639</v>
+        <v>299844</v>
       </c>
       <c r="F35">
         <v>100</v>
@@ -22805,25 +22804,25 @@
         <v>4</v>
       </c>
       <c r="H35" s="18">
-        <f t="shared" si="1"/>
-        <v>5.0455350000000001</v>
+        <f t="shared" ref="H35" si="3">(_xlfn.CEILING.MATH(LOG(D35, 2)))*(B35)*0.000000125</f>
+        <v>4.9787912499999996</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B36">
-        <v>3983033</v>
+        <v>4036428</v>
       </c>
       <c r="C36">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D36">
         <v>912</v>
       </c>
       <c r="E36">
-        <v>299844</v>
+        <v>567639</v>
       </c>
       <c r="F36">
         <v>100</v>
@@ -22832,25 +22831,25 @@
         <v>4</v>
       </c>
       <c r="H36" s="18">
-        <f t="shared" si="1"/>
-        <v>4.9787912499999996</v>
+        <f t="shared" ref="H36" si="4">(_xlfn.CEILING.MATH(LOG(D36, 2)))*(B36)*0.000000125</f>
+        <v>5.0455350000000001</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B37">
-        <v>3918478</v>
+        <v>3733343</v>
       </c>
       <c r="C37">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D37">
-        <v>915</v>
+        <v>908</v>
       </c>
       <c r="E37">
-        <v>150000</v>
+        <v>872472</v>
       </c>
       <c r="F37">
         <v>100</v>
@@ -22859,8 +22858,8 @@
         <v>4</v>
       </c>
       <c r="H37" s="18">
-        <f t="shared" si="1"/>
-        <v>4.8980974999999995</v>
+        <f t="shared" ref="H37" si="5">(_xlfn.CEILING.MATH(LOG(D37, 2)))*(B37)*0.000000125</f>
+        <v>4.66667875</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -23013,7 +23012,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+      <selection activeCell="B7" sqref="B7:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23118,16 +23117,16 @@
         <v>60</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -23135,16 +23134,16 @@
         <v>55</v>
       </c>
       <c r="B8" s="3">
+        <v>1616.71</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3179.241</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4421.4040000000005</v>
+      </c>
+      <c r="E8" s="3">
         <v>1882.4839999999999</v>
-      </c>
-      <c r="C8" s="3">
-        <v>4421.4040000000005</v>
-      </c>
-      <c r="D8" s="3">
-        <v>3179.241</v>
-      </c>
-      <c r="E8" s="3">
-        <v>1616.71</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -23152,16 +23151,16 @@
         <v>56</v>
       </c>
       <c r="B9" s="3">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="D9" s="3">
+        <v>1.3879999999999999</v>
+      </c>
+      <c r="E9" s="3">
         <v>1.4510000000000001</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.3879999999999999</v>
-      </c>
-      <c r="D9" s="3">
-        <v>0.78500000000000003</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.96599999999999997</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -23169,16 +23168,16 @@
         <v>58</v>
       </c>
       <c r="B10" s="3">
+        <v>20.472999999999999</v>
+      </c>
+      <c r="C10" s="3">
+        <v>40.835000000000001</v>
+      </c>
+      <c r="D10" s="3">
+        <v>75.563999999999993</v>
+      </c>
+      <c r="E10" s="3">
         <v>110.43899999999999</v>
-      </c>
-      <c r="C10" s="3">
-        <v>75.563999999999993</v>
-      </c>
-      <c r="D10" s="3">
-        <v>40.835000000000001</v>
-      </c>
-      <c r="E10" s="3">
-        <v>20.472999999999999</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -23300,7 +23299,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="B7" sqref="B7:E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23405,16 +23404,16 @@
         <v>60</v>
       </c>
       <c r="B7" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="E7" s="19" t="s">
         <v>67</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="D7" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="E7" s="19" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -23422,16 +23421,16 @@
         <v>55</v>
       </c>
       <c r="B8" s="18">
+        <v>4.2885</v>
+      </c>
+      <c r="C8" s="18">
+        <v>4.1141300000000003</v>
+      </c>
+      <c r="D8" s="18">
+        <v>4.2238699999999998</v>
+      </c>
+      <c r="E8" s="18">
         <v>4.3745700000000003</v>
-      </c>
-      <c r="C8" s="18">
-        <v>4.2238699999999998</v>
-      </c>
-      <c r="D8" s="18">
-        <v>4.1141300000000003</v>
-      </c>
-      <c r="E8" s="18">
-        <v>4.2885</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -23439,16 +23438,16 @@
         <v>56</v>
       </c>
       <c r="B9" s="18">
+        <v>1.0930200000000001</v>
+      </c>
+      <c r="C9" s="18">
+        <v>0.73525399999999996</v>
+      </c>
+      <c r="D9" s="18">
+        <v>0.36714999999999998</v>
+      </c>
+      <c r="E9" s="18">
         <v>7.2503999999999999E-2</v>
-      </c>
-      <c r="C9" s="18">
-        <v>0.36714999999999998</v>
-      </c>
-      <c r="D9" s="18">
-        <v>0.73525399999999996</v>
-      </c>
-      <c r="E9" s="18">
-        <v>1.0930200000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -23456,16 +23455,16 @@
         <v>58</v>
       </c>
       <c r="B10" s="18">
+        <v>6.96333</v>
+      </c>
+      <c r="C10" s="18">
+        <v>7.07735</v>
+      </c>
+      <c r="D10" s="18">
+        <v>7.2179900000000004</v>
+      </c>
+      <c r="E10" s="18">
         <v>6.6927099999999999</v>
-      </c>
-      <c r="C10" s="18">
-        <v>7.2179900000000004</v>
-      </c>
-      <c r="D10" s="18">
-        <v>7.07735</v>
-      </c>
-      <c r="E10" s="18">
-        <v>6.96333</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="34" x14ac:dyDescent="0.2">
@@ -23586,8 +23585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1854EE8B-C47B-954D-B478-6C02B4ADDC7D}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" zoomScale="91" workbookViewId="0">
-      <selection activeCell="M105" sqref="M105"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="91" workbookViewId="0">
+      <selection activeCell="Z125" sqref="Z125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>